<commit_message>
Updated with last status
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1108">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -4862,6 +4862,114 @@
   </si>
   <si>
     <t>75b4591</t>
+  </si>
+  <si>
+    <t>d0c7be1</t>
+  </si>
+  <si>
+    <t>20d86d5</t>
+  </si>
+  <si>
+    <t>51aec83</t>
+  </si>
+  <si>
+    <t>7725cef</t>
+  </si>
+  <si>
+    <t>7134637</t>
+  </si>
+  <si>
+    <t>f51367c</t>
+  </si>
+  <si>
+    <t>e47bf31</t>
+  </si>
+  <si>
+    <t>1267293</t>
+  </si>
+  <si>
+    <t>adf7641</t>
+  </si>
+  <si>
+    <t>ad17397</t>
+  </si>
+  <si>
+    <t>6421049</t>
+  </si>
+  <si>
+    <t>6a434ae</t>
+  </si>
+  <si>
+    <t>517b2a1</t>
+  </si>
+  <si>
+    <t>31e9d45</t>
+  </si>
+  <si>
+    <t>Can't be an invalid date</t>
+  </si>
+  <si>
+    <t>Can't be an invalid double</t>
+  </si>
+  <si>
+    <t>Can't be an invalid integer</t>
+  </si>
+  <si>
+    <t>f8055ae</t>
+  </si>
+  <si>
+    <t>8b2c7d0</t>
+  </si>
+  <si>
+    <t>7b3864b</t>
+  </si>
+  <si>
+    <t>e32e5b1</t>
+  </si>
+  <si>
+    <t>89c30cc</t>
+  </si>
+  <si>
+    <t>4336e38</t>
+  </si>
+  <si>
+    <t>a2ca2ba</t>
+  </si>
+  <si>
+    <t>29a66d6</t>
+  </si>
+  <si>
+    <t>a2f8105</t>
+  </si>
+  <si>
+    <t>non-sensical rule</t>
+  </si>
+  <si>
+    <t>c4ef31c</t>
+  </si>
+  <si>
+    <t>6fc39e6</t>
+  </si>
+  <si>
+    <t>82de551</t>
+  </si>
+  <si>
+    <t>76d2093</t>
+  </si>
+  <si>
+    <t>94a7284</t>
+  </si>
+  <si>
+    <t>ef602f1</t>
+  </si>
+  <si>
+    <t>8660c3a</t>
+  </si>
+  <si>
+    <t>6200b0d</t>
+  </si>
+  <si>
+    <t>d4e9928</t>
   </si>
 </sst>
 </file>
@@ -4911,7 +5019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4929,6 +5037,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9518,7 +9627,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F308" sqref="F308"/>
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9869,41 +9978,47 @@
     </row>
     <row r="19" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>450</v>
+        <v>656</v>
       </c>
       <c r="B19" t="s">
-        <v>451</v>
+        <v>657</v>
       </c>
       <c r="C19" t="s">
-        <v>462</v>
+        <v>667</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>463</v>
+        <v>659</v>
       </c>
       <c r="E19" t="s">
         <v>464</v>
       </c>
+      <c r="F19" t="s">
+        <v>984</v>
+      </c>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B20" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="C20" t="s">
         <v>462</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E20" t="s">
         <v>464</v>
       </c>
+      <c r="F20" t="s">
+        <v>1089</v>
+      </c>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>465</v>
       </c>
@@ -9911,265 +10026,316 @@
         <v>466</v>
       </c>
       <c r="C21" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E21" t="s">
         <v>464</v>
       </c>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>984</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>465</v>
+        <v>478</v>
       </c>
       <c r="B22" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="C22" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="E22" t="s">
         <v>464</v>
       </c>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>984</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>465</v>
+        <v>488</v>
       </c>
       <c r="B23" t="s">
-        <v>466</v>
+        <v>489</v>
       </c>
       <c r="C23" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>473</v>
+        <v>490</v>
       </c>
       <c r="E23" t="s">
         <v>464</v>
       </c>
+      <c r="F23" t="s">
+        <v>1089</v>
+      </c>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>465</v>
+        <v>656</v>
       </c>
       <c r="B24" t="s">
-        <v>466</v>
+        <v>657</v>
       </c>
       <c r="C24" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>475</v>
+        <v>659</v>
       </c>
       <c r="E24" t="s">
         <v>464</v>
       </c>
+      <c r="F24" t="s">
+        <v>984</v>
+      </c>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>465</v>
+        <v>704</v>
       </c>
       <c r="B25" t="s">
-        <v>466</v>
+        <v>705</v>
       </c>
       <c r="C25" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>477</v>
+        <v>706</v>
       </c>
       <c r="E25" t="s">
         <v>464</v>
       </c>
+      <c r="F25" t="s">
+        <v>1089</v>
+      </c>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>478</v>
+        <v>720</v>
       </c>
       <c r="B26" t="s">
-        <v>479</v>
+        <v>721</v>
       </c>
       <c r="C26" t="s">
         <v>462</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>480</v>
+        <v>724</v>
       </c>
       <c r="E26" t="s">
         <v>464</v>
       </c>
-      <c r="G26"/>
-    </row>
-    <row r="27" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>984</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>478</v>
+        <v>738</v>
       </c>
       <c r="B27" t="s">
-        <v>479</v>
+        <v>739</v>
       </c>
       <c r="C27" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>481</v>
+        <v>740</v>
       </c>
       <c r="E27" t="s">
         <v>464</v>
       </c>
+      <c r="F27" t="s">
+        <v>1089</v>
+      </c>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>478</v>
+        <v>748</v>
       </c>
       <c r="B28" t="s">
-        <v>479</v>
+        <v>749</v>
       </c>
       <c r="C28" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>483</v>
+        <v>750</v>
       </c>
       <c r="E28" t="s">
         <v>464</v>
       </c>
+      <c r="F28" t="s">
+        <v>1089</v>
+      </c>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>478</v>
+        <v>783</v>
       </c>
       <c r="B29" t="s">
-        <v>479</v>
+        <v>784</v>
       </c>
       <c r="C29" t="s">
-        <v>484</v>
+        <v>462</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>485</v>
+        <v>785</v>
       </c>
       <c r="E29" t="s">
         <v>464</v>
       </c>
+      <c r="F29" t="s">
+        <v>1089</v>
+      </c>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="B30" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="C30" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="E30" t="s">
         <v>464</v>
       </c>
+      <c r="F30" t="s">
+        <v>1090</v>
+      </c>
       <c r="G30"/>
     </row>
-    <row r="31" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>488</v>
+        <v>783</v>
       </c>
       <c r="B31" t="s">
-        <v>489</v>
+        <v>784</v>
       </c>
       <c r="C31" t="s">
-        <v>462</v>
+        <v>786</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>490</v>
+        <v>787</v>
       </c>
       <c r="E31" t="s">
         <v>464</v>
       </c>
+      <c r="F31" t="s">
+        <v>1091</v>
+      </c>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="B32" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="C32" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="E32" t="s">
         <v>464</v>
       </c>
+      <c r="F32" t="s">
+        <v>1092</v>
+      </c>
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>488</v>
+        <v>720</v>
       </c>
       <c r="B33" t="s">
-        <v>489</v>
+        <v>721</v>
       </c>
       <c r="C33" t="s">
-        <v>482</v>
+        <v>725</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>492</v>
+        <v>726</v>
       </c>
       <c r="E33" t="s">
         <v>464</v>
       </c>
+      <c r="F33" t="s">
+        <v>1093</v>
+      </c>
       <c r="G33"/>
     </row>
-    <row r="34" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>488</v>
+        <v>720</v>
       </c>
       <c r="B34" t="s">
-        <v>489</v>
+        <v>721</v>
       </c>
       <c r="C34" t="s">
-        <v>484</v>
+        <v>727</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>493</v>
+        <v>728</v>
       </c>
       <c r="E34" t="s">
         <v>464</v>
       </c>
+      <c r="F34" s="9" t="s">
+        <v>1094</v>
+      </c>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="B35" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="C35" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="E35" t="s">
         <v>464</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1095</v>
       </c>
       <c r="G35"/>
     </row>
@@ -11854,21 +12020,24 @@
         <v>984</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>656</v>
+        <v>478</v>
       </c>
       <c r="B129" t="s">
-        <v>657</v>
+        <v>479</v>
       </c>
       <c r="C129" t="s">
-        <v>667</v>
+        <v>472</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>659</v>
+        <v>481</v>
       </c>
       <c r="E129" t="s">
         <v>464</v>
+      </c>
+      <c r="F129" t="s">
+        <v>1095</v>
       </c>
       <c r="G129"/>
     </row>
@@ -11911,21 +12080,24 @@
       </c>
       <c r="G131"/>
     </row>
-    <row r="132" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>656</v>
+        <v>488</v>
       </c>
       <c r="B132" t="s">
-        <v>657</v>
+        <v>489</v>
       </c>
       <c r="C132" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>659</v>
+        <v>491</v>
       </c>
       <c r="E132" t="s">
         <v>464</v>
+      </c>
+      <c r="F132" t="s">
+        <v>1095</v>
       </c>
       <c r="G132"/>
     </row>
@@ -12397,7 +12569,7 @@
       </c>
       <c r="G155"/>
     </row>
-    <row r="156" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>704</v>
       </c>
@@ -12405,107 +12577,125 @@
         <v>705</v>
       </c>
       <c r="C156" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="E156" t="s">
         <v>464</v>
       </c>
+      <c r="F156" t="s">
+        <v>1095</v>
+      </c>
       <c r="G156"/>
     </row>
-    <row r="157" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>704</v>
+        <v>720</v>
       </c>
       <c r="B157" t="s">
-        <v>705</v>
+        <v>721</v>
       </c>
       <c r="C157" t="s">
         <v>472</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>707</v>
+        <v>729</v>
       </c>
       <c r="E157" t="s">
         <v>464</v>
       </c>
+      <c r="F157" t="s">
+        <v>1095</v>
+      </c>
       <c r="G157"/>
     </row>
-    <row r="158" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>704</v>
+        <v>738</v>
       </c>
       <c r="B158" t="s">
-        <v>705</v>
+        <v>739</v>
       </c>
       <c r="C158" t="s">
-        <v>708</v>
+        <v>472</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>709</v>
+        <v>741</v>
       </c>
       <c r="E158" t="s">
         <v>464</v>
       </c>
+      <c r="F158" t="s">
+        <v>1095</v>
+      </c>
       <c r="G158"/>
     </row>
-    <row r="159" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>704</v>
+        <v>748</v>
       </c>
       <c r="B159" t="s">
-        <v>705</v>
+        <v>749</v>
       </c>
       <c r="C159" t="s">
-        <v>710</v>
+        <v>472</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>711</v>
+        <v>751</v>
       </c>
       <c r="E159" t="s">
         <v>464</v>
       </c>
+      <c r="F159" t="s">
+        <v>1095</v>
+      </c>
       <c r="G159"/>
     </row>
-    <row r="160" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>704</v>
+        <v>783</v>
       </c>
       <c r="B160" t="s">
-        <v>705</v>
+        <v>784</v>
       </c>
       <c r="C160" t="s">
-        <v>712</v>
+        <v>472</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>713</v>
+        <v>788</v>
       </c>
       <c r="E160" t="s">
         <v>464</v>
       </c>
+      <c r="F160" t="s">
+        <v>1095</v>
+      </c>
       <c r="G160"/>
     </row>
-    <row r="161" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>704</v>
+        <v>720</v>
       </c>
       <c r="B161" t="s">
-        <v>705</v>
+        <v>721</v>
       </c>
       <c r="C161" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>715</v>
+        <v>731</v>
       </c>
       <c r="E161" t="s">
         <v>464</v>
       </c>
+      <c r="F161" t="s">
+        <v>1096</v>
+      </c>
       <c r="G161"/>
     </row>
-    <row r="162" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>704</v>
       </c>
@@ -12513,31 +12703,37 @@
         <v>705</v>
       </c>
       <c r="C162" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="E162" t="s">
         <v>464</v>
       </c>
+      <c r="F162" t="s">
+        <v>1097</v>
+      </c>
       <c r="G162"/>
     </row>
-    <row r="163" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>704</v>
+        <v>465</v>
       </c>
       <c r="B163" t="s">
-        <v>705</v>
+        <v>466</v>
       </c>
       <c r="C163" t="s">
-        <v>718</v>
+        <v>474</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>719</v>
+        <v>475</v>
       </c>
       <c r="E163" t="s">
         <v>464</v>
+      </c>
+      <c r="F163" t="s">
+        <v>1099</v>
       </c>
       <c r="G163"/>
     </row>
@@ -12561,23 +12757,28 @@
     </row>
     <row r="165" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="B165" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
       <c r="C165" t="s">
-        <v>462</v>
+        <v>710</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="E165" t="s">
         <v>464</v>
       </c>
-      <c r="G165"/>
-    </row>
-    <row r="166" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F165" t="s">
+        <v>984</v>
+      </c>
+      <c r="G165" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>720</v>
       </c>
@@ -12585,316 +12786,357 @@
         <v>721</v>
       </c>
       <c r="C166" t="s">
-        <v>725</v>
+        <v>710</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="E166" t="s">
         <v>464</v>
       </c>
-      <c r="G166"/>
-    </row>
-    <row r="167" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F166" t="s">
+        <v>984</v>
+      </c>
+      <c r="G166" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>720</v>
+        <v>738</v>
       </c>
       <c r="B167" t="s">
-        <v>721</v>
+        <v>739</v>
       </c>
       <c r="C167" t="s">
-        <v>727</v>
+        <v>742</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>728</v>
+        <v>743</v>
       </c>
       <c r="E167" t="s">
         <v>464</v>
       </c>
+      <c r="F167" t="s">
+        <v>1100</v>
+      </c>
       <c r="G167"/>
     </row>
-    <row r="168" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>720</v>
+        <v>738</v>
       </c>
       <c r="B168" t="s">
-        <v>721</v>
+        <v>739</v>
       </c>
       <c r="C168" t="s">
-        <v>472</v>
+        <v>744</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>729</v>
+        <v>745</v>
       </c>
       <c r="E168" t="s">
         <v>464</v>
       </c>
+      <c r="F168" t="s">
+        <v>1101</v>
+      </c>
       <c r="G168"/>
     </row>
-    <row r="169" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="B169" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
       <c r="C169" t="s">
-        <v>730</v>
+        <v>712</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>731</v>
+        <v>713</v>
       </c>
       <c r="E169" t="s">
         <v>464</v>
       </c>
+      <c r="F169" t="s">
+        <v>1102</v>
+      </c>
       <c r="G169"/>
     </row>
-    <row r="170" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>720</v>
+        <v>748</v>
       </c>
       <c r="B170" t="s">
-        <v>721</v>
+        <v>749</v>
       </c>
       <c r="C170" t="s">
-        <v>710</v>
+        <v>752</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>732</v>
+        <v>753</v>
       </c>
       <c r="E170" t="s">
         <v>464</v>
       </c>
+      <c r="F170" t="s">
+        <v>1103</v>
+      </c>
       <c r="G170"/>
     </row>
     <row r="171" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>720</v>
+        <v>748</v>
       </c>
       <c r="B171" t="s">
-        <v>721</v>
+        <v>749</v>
       </c>
       <c r="C171" t="s">
-        <v>476</v>
+        <v>754</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>733</v>
+        <v>755</v>
       </c>
       <c r="E171" t="s">
         <v>464</v>
       </c>
+      <c r="F171" t="s">
+        <v>1103</v>
+      </c>
       <c r="G171"/>
     </row>
-    <row r="172" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>720</v>
+        <v>783</v>
       </c>
       <c r="B172" t="s">
-        <v>721</v>
+        <v>784</v>
       </c>
       <c r="C172" t="s">
-        <v>734</v>
+        <v>789</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>735</v>
+        <v>790</v>
       </c>
       <c r="E172" t="s">
         <v>464</v>
       </c>
+      <c r="F172" t="s">
+        <v>1104</v>
+      </c>
       <c r="G172"/>
     </row>
-    <row r="173" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>720</v>
+        <v>478</v>
       </c>
       <c r="B173" t="s">
-        <v>721</v>
+        <v>479</v>
       </c>
       <c r="C173" t="s">
-        <v>736</v>
+        <v>482</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>737</v>
+        <v>483</v>
       </c>
       <c r="E173" t="s">
         <v>464</v>
       </c>
+      <c r="F173" t="s">
+        <v>1105</v>
+      </c>
       <c r="G173"/>
     </row>
     <row r="174" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>738</v>
+        <v>488</v>
       </c>
       <c r="B174" t="s">
-        <v>739</v>
+        <v>489</v>
       </c>
       <c r="C174" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>740</v>
+        <v>492</v>
       </c>
       <c r="E174" t="s">
         <v>464</v>
       </c>
+      <c r="F174" t="s">
+        <v>1105</v>
+      </c>
       <c r="G174"/>
     </row>
-    <row r="175" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>738</v>
+        <v>478</v>
       </c>
       <c r="B175" t="s">
-        <v>739</v>
+        <v>479</v>
       </c>
       <c r="C175" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>741</v>
+        <v>485</v>
       </c>
       <c r="E175" t="s">
         <v>464</v>
       </c>
+      <c r="F175" t="s">
+        <v>1106</v>
+      </c>
       <c r="G175"/>
     </row>
-    <row r="176" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>738</v>
+        <v>488</v>
       </c>
       <c r="B176" t="s">
-        <v>739</v>
+        <v>489</v>
       </c>
       <c r="C176" t="s">
-        <v>742</v>
+        <v>484</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>743</v>
+        <v>493</v>
       </c>
       <c r="E176" t="s">
         <v>464</v>
       </c>
+      <c r="F176" t="s">
+        <v>1106</v>
+      </c>
       <c r="G176"/>
     </row>
     <row r="177" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>738</v>
+        <v>783</v>
       </c>
       <c r="B177" t="s">
-        <v>739</v>
+        <v>784</v>
       </c>
       <c r="C177" t="s">
-        <v>744</v>
+        <v>484</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>745</v>
+        <v>791</v>
       </c>
       <c r="E177" t="s">
         <v>464</v>
       </c>
+      <c r="F177" t="s">
+        <v>1106</v>
+      </c>
       <c r="G177"/>
     </row>
-    <row r="178" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>738</v>
+        <v>488</v>
       </c>
       <c r="B178" t="s">
-        <v>739</v>
+        <v>489</v>
       </c>
       <c r="C178" t="s">
-        <v>746</v>
+        <v>494</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>747</v>
+        <v>495</v>
       </c>
       <c r="E178" t="s">
         <v>464</v>
       </c>
+      <c r="F178" t="s">
+        <v>1107</v>
+      </c>
       <c r="G178"/>
     </row>
-    <row r="179" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>748</v>
+        <v>465</v>
       </c>
       <c r="B179" t="s">
-        <v>749</v>
+        <v>466</v>
       </c>
       <c r="C179" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>750</v>
+        <v>477</v>
       </c>
       <c r="E179" t="s">
         <v>464</v>
       </c>
       <c r="G179"/>
     </row>
-    <row r="180" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>748</v>
+        <v>720</v>
       </c>
       <c r="B180" t="s">
-        <v>749</v>
+        <v>721</v>
       </c>
       <c r="C180" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>751</v>
+        <v>733</v>
       </c>
       <c r="E180" t="s">
         <v>464</v>
       </c>
       <c r="G180"/>
     </row>
-    <row r="181" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>748</v>
+        <v>704</v>
       </c>
       <c r="B181" t="s">
-        <v>749</v>
+        <v>705</v>
       </c>
       <c r="C181" t="s">
-        <v>752</v>
+        <v>714</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>753</v>
+        <v>715</v>
       </c>
       <c r="E181" t="s">
         <v>464</v>
       </c>
       <c r="G181"/>
     </row>
-    <row r="182" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>748</v>
+        <v>720</v>
       </c>
       <c r="B182" t="s">
-        <v>749</v>
+        <v>721</v>
       </c>
       <c r="C182" t="s">
-        <v>754</v>
+        <v>734</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>755</v>
+        <v>735</v>
       </c>
       <c r="E182" t="s">
         <v>464</v>
       </c>
       <c r="G182"/>
     </row>
-    <row r="183" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>748</v>
+        <v>478</v>
       </c>
       <c r="B183" t="s">
-        <v>749</v>
+        <v>479</v>
       </c>
       <c r="C183" t="s">
-        <v>756</v>
+        <v>486</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>757</v>
+        <v>487</v>
       </c>
       <c r="E183" t="s">
         <v>464</v>
@@ -13153,6 +13395,9 @@
       <c r="E196" t="s">
         <v>464</v>
       </c>
+      <c r="F196" t="s">
+        <v>984</v>
+      </c>
       <c r="G196"/>
     </row>
     <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -13171,6 +13416,9 @@
       <c r="E197" t="s">
         <v>464</v>
       </c>
+      <c r="F197" t="s">
+        <v>984</v>
+      </c>
       <c r="G197"/>
     </row>
     <row r="198" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -13189,6 +13437,9 @@
       <c r="E198" t="s">
         <v>464</v>
       </c>
+      <c r="F198" t="s">
+        <v>984</v>
+      </c>
       <c r="G198"/>
     </row>
     <row r="199" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -13207,6 +13458,9 @@
       <c r="E199" t="s">
         <v>464</v>
       </c>
+      <c r="F199" t="s">
+        <v>984</v>
+      </c>
       <c r="G199"/>
     </row>
     <row r="200" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -13425,97 +13679,100 @@
       </c>
       <c r="G211"/>
     </row>
-    <row r="212" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>783</v>
+        <v>704</v>
       </c>
       <c r="B212" t="s">
-        <v>784</v>
+        <v>705</v>
       </c>
       <c r="C212" t="s">
-        <v>462</v>
+        <v>716</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>785</v>
+        <v>717</v>
       </c>
       <c r="E212" t="s">
         <v>464</v>
       </c>
       <c r="G212"/>
     </row>
-    <row r="213" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>783</v>
+        <v>738</v>
       </c>
       <c r="B213" t="s">
-        <v>784</v>
+        <v>739</v>
       </c>
       <c r="C213" t="s">
-        <v>786</v>
+        <v>746</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>787</v>
+        <v>747</v>
       </c>
       <c r="E213" t="s">
         <v>464</v>
       </c>
       <c r="G213"/>
     </row>
-    <row r="214" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>783</v>
+        <v>748</v>
       </c>
       <c r="B214" t="s">
-        <v>784</v>
+        <v>749</v>
       </c>
       <c r="C214" t="s">
-        <v>472</v>
+        <v>756</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>788</v>
+        <v>757</v>
       </c>
       <c r="E214" t="s">
         <v>464</v>
       </c>
       <c r="G214"/>
     </row>
-    <row r="215" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>783</v>
+        <v>704</v>
       </c>
       <c r="B215" t="s">
-        <v>784</v>
+        <v>705</v>
       </c>
       <c r="C215" t="s">
-        <v>789</v>
+        <v>718</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>790</v>
+        <v>719</v>
       </c>
       <c r="E215" t="s">
         <v>464</v>
       </c>
       <c r="G215"/>
     </row>
-    <row r="216" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>783</v>
+        <v>720</v>
       </c>
       <c r="B216" t="s">
-        <v>784</v>
+        <v>721</v>
       </c>
       <c r="C216" t="s">
-        <v>484</v>
+        <v>736</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>791</v>
+        <v>737</v>
       </c>
       <c r="E216" t="s">
         <v>464</v>
       </c>
+      <c r="F216" s="9" t="s">
+        <v>1094</v>
+      </c>
       <c r="G216"/>
     </row>
-    <row r="217" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>783</v>
       </c>
@@ -15204,7 +15461,7 @@
       </c>
       <c r="G307"/>
     </row>
-    <row r="308" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>687</v>
       </c>
@@ -15220,9 +15477,12 @@
       <c r="E308" t="s">
         <v>445</v>
       </c>
+      <c r="F308" t="s">
+        <v>1072</v>
+      </c>
       <c r="G308"/>
     </row>
-    <row r="309" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>957</v>
       </c>
@@ -15238,9 +15498,12 @@
       <c r="E309" t="s">
         <v>445</v>
       </c>
+      <c r="F309" t="s">
+        <v>1073</v>
+      </c>
       <c r="G309"/>
     </row>
-    <row r="310" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>441</v>
       </c>
@@ -15256,9 +15519,12 @@
       <c r="E310" t="s">
         <v>445</v>
       </c>
+      <c r="F310" t="s">
+        <v>1074</v>
+      </c>
       <c r="G310"/>
     </row>
-    <row r="311" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>669</v>
       </c>
@@ -15274,9 +15540,12 @@
       <c r="E311" t="s">
         <v>445</v>
       </c>
+      <c r="F311" t="s">
+        <v>1075</v>
+      </c>
       <c r="G311"/>
     </row>
-    <row r="312" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>669</v>
       </c>
@@ -15292,9 +15561,12 @@
       <c r="E312" t="s">
         <v>445</v>
       </c>
+      <c r="F312" s="3" t="s">
+        <v>1076</v>
+      </c>
       <c r="G312"/>
     </row>
-    <row r="313" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>687</v>
       </c>
@@ -15310,9 +15582,12 @@
       <c r="E313" t="s">
         <v>445</v>
       </c>
+      <c r="F313" t="s">
+        <v>1077</v>
+      </c>
       <c r="G313"/>
     </row>
-    <row r="314" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>957</v>
       </c>
@@ -15328,9 +15603,12 @@
       <c r="E314" t="s">
         <v>445</v>
       </c>
+      <c r="F314" t="s">
+        <v>1078</v>
+      </c>
       <c r="G314"/>
     </row>
-    <row r="315" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>441</v>
       </c>
@@ -15346,9 +15624,12 @@
       <c r="E315" t="s">
         <v>445</v>
       </c>
+      <c r="F315" s="3" t="s">
+        <v>1079</v>
+      </c>
       <c r="G315"/>
     </row>
-    <row r="316" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>687</v>
       </c>
@@ -15364,9 +15645,12 @@
       <c r="E316" t="s">
         <v>445</v>
       </c>
+      <c r="F316" t="s">
+        <v>1080</v>
+      </c>
       <c r="G316"/>
     </row>
-    <row r="317" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>953</v>
       </c>
@@ -15382,9 +15666,12 @@
       <c r="E317" t="s">
         <v>445</v>
       </c>
+      <c r="F317" t="s">
+        <v>1081</v>
+      </c>
       <c r="G317"/>
     </row>
-    <row r="318" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>687</v>
       </c>
@@ -15400,9 +15687,12 @@
       <c r="E318" t="s">
         <v>445</v>
       </c>
+      <c r="F318" s="3" t="s">
+        <v>1082</v>
+      </c>
       <c r="G318"/>
     </row>
-    <row r="319" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>687</v>
       </c>
@@ -15418,9 +15708,12 @@
       <c r="E319" t="s">
         <v>445</v>
       </c>
+      <c r="F319" t="s">
+        <v>1083</v>
+      </c>
       <c r="G319"/>
     </row>
-    <row r="320" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>687</v>
       </c>
@@ -15436,9 +15729,12 @@
       <c r="E320" t="s">
         <v>445</v>
       </c>
+      <c r="F320" t="s">
+        <v>1084</v>
+      </c>
       <c r="G320"/>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>968</v>
       </c>
@@ -15453,6 +15749,9 @@
       </c>
       <c r="E321" t="s">
         <v>445</v>
+      </c>
+      <c r="F321" t="s">
+        <v>1085</v>
       </c>
       <c r="G321"/>
     </row>
@@ -15917,13 +16216,13 @@
   <autoFilter ref="A1:G345">
     <filterColumn colId="4">
       <filters>
-        <filter val="2"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A308:G321">
+    <sortState ref="A179:G217">
       <sortCondition ref="C8"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
updated spreadsheet for victim rules unit tests
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="1111">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -4977,7 +4977,16 @@
     <t>d4e9928</t>
   </si>
   <si>
-    <t>0a2055d</t>
+    <t>0a2055d
+factory test: 936f6d7</t>
+  </si>
+  <si>
+    <t>0a2055d
+factory test: 56069d2</t>
+  </si>
+  <si>
+    <t>0a2055d
+facbory test: 56069d2</t>
   </si>
 </sst>
 </file>
@@ -9672,20 +9681,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="F171" sqref="C167:F171"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167:F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9709,7 +9719,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" hidden="1">
       <c r="A2" t="s">
         <v>656</v>
       </c>
@@ -9727,7 +9737,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="28">
+    <row r="3" spans="1:7" ht="28" hidden="1">
       <c r="A3" t="s">
         <v>758</v>
       </c>
@@ -9745,7 +9755,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4" t="s">
         <v>990</v>
       </c>
@@ -9763,7 +9773,7 @@
       </c>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" ht="28">
+    <row r="5" spans="1:7" ht="28" hidden="1">
       <c r="A5" t="s">
         <v>991</v>
       </c>
@@ -9781,7 +9791,7 @@
       </c>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" ht="28">
+    <row r="6" spans="1:7" ht="28" hidden="1">
       <c r="A6" t="s">
         <v>992</v>
       </c>
@@ -9799,7 +9809,7 @@
       </c>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" ht="28">
+    <row r="7" spans="1:7" ht="28" hidden="1">
       <c r="A7" t="s">
         <v>991</v>
       </c>
@@ -9817,7 +9827,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" ht="28">
+    <row r="8" spans="1:7" ht="28" hidden="1">
       <c r="A8" t="s">
         <v>990</v>
       </c>
@@ -9835,7 +9845,7 @@
       </c>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" ht="28">
+    <row r="9" spans="1:7" ht="28" hidden="1">
       <c r="A9" t="s">
         <v>656</v>
       </c>
@@ -9853,7 +9863,7 @@
       </c>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7" ht="28">
+    <row r="10" spans="1:7" ht="28" hidden="1">
       <c r="A10" t="s">
         <v>818</v>
       </c>
@@ -9871,7 +9881,7 @@
       </c>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" ht="42">
+    <row r="11" spans="1:7" ht="42" hidden="1">
       <c r="A11" t="s">
         <v>758</v>
       </c>
@@ -9889,7 +9899,7 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" ht="28">
+    <row r="12" spans="1:7" ht="28" hidden="1">
       <c r="A12" t="s">
         <v>656</v>
       </c>
@@ -9907,7 +9917,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" ht="42">
+    <row r="13" spans="1:7" ht="42" hidden="1">
       <c r="A13" t="s">
         <v>450</v>
       </c>
@@ -9925,7 +9935,7 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" ht="28">
+    <row r="14" spans="1:7" ht="28" hidden="1">
       <c r="A14" t="s">
         <v>450</v>
       </c>
@@ -9943,7 +9953,7 @@
       </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:7" ht="42">
+    <row r="15" spans="1:7" ht="42" hidden="1">
       <c r="A15" t="s">
         <v>450</v>
       </c>
@@ -9961,7 +9971,7 @@
       </c>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:7" ht="42">
+    <row r="16" spans="1:7" ht="42" hidden="1">
       <c r="A16" t="s">
         <v>450</v>
       </c>
@@ -9979,7 +9989,7 @@
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" ht="42">
+    <row r="17" spans="1:7" ht="42" hidden="1">
       <c r="A17" t="s">
         <v>450</v>
       </c>
@@ -9997,7 +10007,7 @@
       </c>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" ht="280">
+    <row r="18" spans="1:7" ht="280" hidden="1">
       <c r="A18" t="s">
         <v>450</v>
       </c>
@@ -10015,7 +10025,7 @@
       </c>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" t="s">
         <v>450</v>
       </c>
@@ -10033,7 +10043,7 @@
       </c>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" ht="28">
+    <row r="20" spans="1:7" ht="28" hidden="1">
       <c r="A20" t="s">
         <v>450</v>
       </c>
@@ -10051,7 +10061,7 @@
       </c>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" ht="28">
+    <row r="21" spans="1:7" ht="28" hidden="1">
       <c r="A21" t="s">
         <v>720</v>
       </c>
@@ -10069,7 +10079,7 @@
       </c>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" ht="28">
+    <row r="22" spans="1:7" ht="28" hidden="1">
       <c r="A22" t="s">
         <v>656</v>
       </c>
@@ -10087,7 +10097,7 @@
       </c>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" ht="28">
+    <row r="23" spans="1:7" ht="28" hidden="1">
       <c r="A23" t="s">
         <v>758</v>
       </c>
@@ -10105,7 +10115,7 @@
       </c>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" t="s">
         <v>758</v>
       </c>
@@ -10123,7 +10133,7 @@
       </c>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" ht="28">
+    <row r="25" spans="1:7" ht="28" hidden="1">
       <c r="A25" t="s">
         <v>989</v>
       </c>
@@ -10141,7 +10151,7 @@
       </c>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" ht="28">
+    <row r="26" spans="1:7" ht="28" hidden="1">
       <c r="A26" t="s">
         <v>1041</v>
       </c>
@@ -10159,7 +10169,7 @@
       </c>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" ht="28">
+    <row r="27" spans="1:7" ht="28" hidden="1">
       <c r="A27" t="s">
         <v>1043</v>
       </c>
@@ -10177,7 +10187,7 @@
       </c>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" ht="28">
+    <row r="28" spans="1:7" ht="28" hidden="1">
       <c r="A28" t="s">
         <v>990</v>
       </c>
@@ -10198,7 +10208,7 @@
       </c>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="28">
+    <row r="29" spans="1:7" ht="28" hidden="1">
       <c r="A29" t="s">
         <v>991</v>
       </c>
@@ -10219,7 +10229,7 @@
       </c>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" ht="84">
+    <row r="30" spans="1:7" ht="84" hidden="1">
       <c r="A30" t="s">
         <v>986</v>
       </c>
@@ -10239,7 +10249,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="126">
+    <row r="31" spans="1:7" ht="126" hidden="1">
       <c r="A31" t="s">
         <v>987</v>
       </c>
@@ -10259,7 +10269,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="70">
+    <row r="32" spans="1:7" ht="70" hidden="1">
       <c r="A32" t="s">
         <v>990</v>
       </c>
@@ -10277,7 +10287,7 @@
       </c>
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:7" ht="70">
+    <row r="33" spans="1:7" ht="70" hidden="1">
       <c r="A33" t="s">
         <v>991</v>
       </c>
@@ -10295,7 +10305,7 @@
       </c>
       <c r="G33"/>
     </row>
-    <row r="34" spans="1:7" ht="140">
+    <row r="34" spans="1:7" ht="140" hidden="1">
       <c r="A34" t="s">
         <v>991</v>
       </c>
@@ -10316,7 +10326,7 @@
       </c>
       <c r="G34"/>
     </row>
-    <row r="35" spans="1:7" ht="98">
+    <row r="35" spans="1:7" ht="98" hidden="1">
       <c r="A35" t="s">
         <v>656</v>
       </c>
@@ -10336,7 +10346,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="28">
+    <row r="36" spans="1:7" ht="28" hidden="1">
       <c r="A36" t="s">
         <v>758</v>
       </c>
@@ -10356,7 +10366,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="28">
+    <row r="37" spans="1:7" ht="28" hidden="1">
       <c r="A37" t="s">
         <v>841</v>
       </c>
@@ -10376,7 +10386,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="28">
+    <row r="38" spans="1:7" ht="28" hidden="1">
       <c r="A38" t="s">
         <v>1045</v>
       </c>
@@ -10394,7 +10404,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="1:7" ht="210">
+    <row r="39" spans="1:7" ht="210" hidden="1">
       <c r="A39" t="s">
         <v>907</v>
       </c>
@@ -10414,7 +10424,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="28">
+    <row r="40" spans="1:7" ht="28" hidden="1">
       <c r="A40" t="s">
         <v>986</v>
       </c>
@@ -10434,7 +10444,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" t="s">
         <v>987</v>
       </c>
@@ -10454,7 +10464,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28">
+    <row r="42" spans="1:7" ht="28" hidden="1">
       <c r="A42" t="s">
         <v>988</v>
       </c>
@@ -10474,7 +10484,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" t="s">
         <v>988</v>
       </c>
@@ -10494,7 +10504,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" t="s">
         <v>656</v>
       </c>
@@ -10514,7 +10524,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1">
       <c r="A45" t="s">
         <v>836</v>
       </c>
@@ -10534,7 +10544,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" t="s">
         <v>841</v>
       </c>
@@ -10554,7 +10564,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="42">
+    <row r="47" spans="1:7" ht="42" hidden="1">
       <c r="A47" t="s">
         <v>841</v>
       </c>
@@ -10574,7 +10584,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="28">
+    <row r="48" spans="1:7" ht="28" hidden="1">
       <c r="A48" t="s">
         <v>930</v>
       </c>
@@ -10594,7 +10604,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="42">
+    <row r="49" spans="1:7" ht="42" hidden="1">
       <c r="A49" t="s">
         <v>987</v>
       </c>
@@ -10614,7 +10624,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="28">
+    <row r="50" spans="1:7" ht="28" hidden="1">
       <c r="A50" t="s">
         <v>986</v>
       </c>
@@ -10634,7 +10644,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="42">
+    <row r="51" spans="1:7" ht="42" hidden="1">
       <c r="A51" t="s">
         <v>841</v>
       </c>
@@ -10654,7 +10664,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" t="s">
         <v>930</v>
       </c>
@@ -10677,7 +10687,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="42">
+    <row r="53" spans="1:7" ht="42" hidden="1">
       <c r="A53" t="s">
         <v>758</v>
       </c>
@@ -10697,7 +10707,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="28">
+    <row r="54" spans="1:7" ht="28" hidden="1">
       <c r="A54" t="s">
         <v>758</v>
       </c>
@@ -10717,7 +10727,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28">
+    <row r="55" spans="1:7" ht="28" hidden="1">
       <c r="A55" t="s">
         <v>758</v>
       </c>
@@ -10737,7 +10747,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="280">
+    <row r="56" spans="1:7" ht="280" hidden="1">
       <c r="A56" t="s">
         <v>841</v>
       </c>
@@ -10757,7 +10767,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="56">
+    <row r="57" spans="1:7" ht="56" hidden="1">
       <c r="A57" t="s">
         <v>836</v>
       </c>
@@ -10777,7 +10787,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="42">
+    <row r="58" spans="1:7" ht="42" hidden="1">
       <c r="A58" t="s">
         <v>841</v>
       </c>
@@ -10797,7 +10807,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="56">
+    <row r="59" spans="1:7" ht="56" hidden="1">
       <c r="A59" t="s">
         <v>841</v>
       </c>
@@ -10817,7 +10827,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="56">
+    <row r="60" spans="1:7" ht="56" hidden="1">
       <c r="A60" t="s">
         <v>907</v>
       </c>
@@ -10837,7 +10847,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="28">
+    <row r="61" spans="1:7" ht="28" hidden="1">
       <c r="A61" t="s">
         <v>930</v>
       </c>
@@ -10857,7 +10867,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="28">
+    <row r="62" spans="1:7" ht="28" hidden="1">
       <c r="A62" t="s">
         <v>930</v>
       </c>
@@ -10877,7 +10887,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="56">
+    <row r="63" spans="1:7" ht="56" hidden="1">
       <c r="A63" t="s">
         <v>907</v>
       </c>
@@ -10900,7 +10910,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="42">
+    <row r="64" spans="1:7" ht="42" hidden="1">
       <c r="A64" t="s">
         <v>841</v>
       </c>
@@ -10920,7 +10930,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="28">
+    <row r="65" spans="1:7" ht="28" hidden="1">
       <c r="A65" t="s">
         <v>841</v>
       </c>
@@ -10940,7 +10950,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="28">
+    <row r="66" spans="1:7" ht="28" hidden="1">
       <c r="A66" t="s">
         <v>841</v>
       </c>
@@ -10960,7 +10970,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="28">
+    <row r="67" spans="1:7" ht="28" hidden="1">
       <c r="A67" t="s">
         <v>841</v>
       </c>
@@ -10980,7 +10990,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" hidden="1">
       <c r="A68" t="s">
         <v>930</v>
       </c>
@@ -11000,7 +11010,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="28">
+    <row r="69" spans="1:7" ht="28" hidden="1">
       <c r="A69" t="s">
         <v>953</v>
       </c>
@@ -11021,7 +11031,7 @@
       </c>
       <c r="G69"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" t="s">
         <v>957</v>
       </c>
@@ -11042,7 +11052,7 @@
       </c>
       <c r="G70"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" t="s">
         <v>963</v>
       </c>
@@ -11063,7 +11073,7 @@
       </c>
       <c r="G71"/>
     </row>
-    <row r="72" spans="1:7" ht="28">
+    <row r="72" spans="1:7" ht="28" hidden="1">
       <c r="A72" t="s">
         <v>656</v>
       </c>
@@ -11084,7 +11094,7 @@
       </c>
       <c r="G72"/>
     </row>
-    <row r="73" spans="1:7" ht="28">
+    <row r="73" spans="1:7" ht="28" hidden="1">
       <c r="A73" t="s">
         <v>968</v>
       </c>
@@ -11105,7 +11115,7 @@
       </c>
       <c r="G73"/>
     </row>
-    <row r="74" spans="1:7" ht="70">
+    <row r="74" spans="1:7" ht="70" hidden="1">
       <c r="A74" t="s">
         <v>975</v>
       </c>
@@ -11126,7 +11136,7 @@
       </c>
       <c r="G74"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" hidden="1">
       <c r="A75" t="s">
         <v>758</v>
       </c>
@@ -11147,7 +11157,7 @@
       </c>
       <c r="G75"/>
     </row>
-    <row r="76" spans="1:7" ht="28">
+    <row r="76" spans="1:7" ht="28" hidden="1">
       <c r="A76" t="s">
         <v>656</v>
       </c>
@@ -11168,7 +11178,7 @@
       </c>
       <c r="G76"/>
     </row>
-    <row r="77" spans="1:7" ht="28">
+    <row r="77" spans="1:7" ht="28" hidden="1">
       <c r="A77" t="s">
         <v>441</v>
       </c>
@@ -11189,7 +11199,7 @@
       </c>
       <c r="G77"/>
     </row>
-    <row r="78" spans="1:7" ht="28">
+    <row r="78" spans="1:7" ht="28" hidden="1">
       <c r="A78" t="s">
         <v>669</v>
       </c>
@@ -11210,7 +11220,7 @@
       </c>
       <c r="G78"/>
     </row>
-    <row r="79" spans="1:7" ht="28">
+    <row r="79" spans="1:7" ht="28" hidden="1">
       <c r="A79" t="s">
         <v>676</v>
       </c>
@@ -11231,7 +11241,7 @@
       </c>
       <c r="G79"/>
     </row>
-    <row r="80" spans="1:7" ht="28">
+    <row r="80" spans="1:7" ht="28" hidden="1">
       <c r="A80" t="s">
         <v>687</v>
       </c>
@@ -11252,7 +11262,7 @@
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="1:7" ht="70">
+    <row r="81" spans="1:7" ht="70" hidden="1">
       <c r="A81" t="s">
         <v>687</v>
       </c>
@@ -11273,7 +11283,7 @@
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="1:7" ht="28">
+    <row r="82" spans="1:7" ht="28" hidden="1">
       <c r="A82" t="s">
         <v>968</v>
       </c>
@@ -11294,7 +11304,7 @@
       </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="1:7" ht="28">
+    <row r="83" spans="1:7" ht="28" hidden="1">
       <c r="A83" t="s">
         <v>975</v>
       </c>
@@ -11315,7 +11325,7 @@
       </c>
       <c r="G83"/>
     </row>
-    <row r="84" spans="1:7" ht="28">
+    <row r="84" spans="1:7" ht="28" hidden="1">
       <c r="A84" t="s">
         <v>676</v>
       </c>
@@ -11336,7 +11346,7 @@
       </c>
       <c r="G84"/>
     </row>
-    <row r="85" spans="1:7" ht="70">
+    <row r="85" spans="1:7" ht="70" hidden="1">
       <c r="A85" t="s">
         <v>687</v>
       </c>
@@ -11357,7 +11367,7 @@
       </c>
       <c r="G85"/>
     </row>
-    <row r="86" spans="1:7" ht="28">
+    <row r="86" spans="1:7" ht="28" hidden="1">
       <c r="A86" t="s">
         <v>963</v>
       </c>
@@ -11378,7 +11388,7 @@
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="1:7" ht="28">
+    <row r="87" spans="1:7" ht="28" hidden="1">
       <c r="A87" t="s">
         <v>968</v>
       </c>
@@ -11399,7 +11409,7 @@
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="1:7" ht="28">
+    <row r="88" spans="1:7" ht="28" hidden="1">
       <c r="A88" t="s">
         <v>676</v>
       </c>
@@ -11420,7 +11430,7 @@
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="1:7" ht="28">
+    <row r="89" spans="1:7" ht="28" hidden="1">
       <c r="A89" t="s">
         <v>687</v>
       </c>
@@ -11441,7 +11451,7 @@
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="1:7" ht="28">
+    <row r="90" spans="1:7" ht="28" hidden="1">
       <c r="A90" t="s">
         <v>963</v>
       </c>
@@ -11462,7 +11472,7 @@
       </c>
       <c r="G90"/>
     </row>
-    <row r="91" spans="1:7" ht="28">
+    <row r="91" spans="1:7" ht="28" hidden="1">
       <c r="A91" t="s">
         <v>968</v>
       </c>
@@ -11483,7 +11493,7 @@
       </c>
       <c r="G91"/>
     </row>
-    <row r="92" spans="1:7" ht="28">
+    <row r="92" spans="1:7" ht="28" hidden="1">
       <c r="A92" t="s">
         <v>758</v>
       </c>
@@ -11504,7 +11514,7 @@
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="1:7" ht="28">
+    <row r="93" spans="1:7" ht="28" hidden="1">
       <c r="A93" t="s">
         <v>758</v>
       </c>
@@ -11525,7 +11535,7 @@
       </c>
       <c r="G93"/>
     </row>
-    <row r="94" spans="1:7" ht="28">
+    <row r="94" spans="1:7" ht="28" hidden="1">
       <c r="A94" t="s">
         <v>758</v>
       </c>
@@ -11546,7 +11556,7 @@
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="1:7" ht="28">
+    <row r="95" spans="1:7" ht="28" hidden="1">
       <c r="A95" t="s">
         <v>676</v>
       </c>
@@ -11567,7 +11577,7 @@
       </c>
       <c r="G95"/>
     </row>
-    <row r="96" spans="1:7" ht="28">
+    <row r="96" spans="1:7" ht="28" hidden="1">
       <c r="A96" t="s">
         <v>676</v>
       </c>
@@ -11588,7 +11598,7 @@
       </c>
       <c r="G96"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" hidden="1">
       <c r="A97" t="s">
         <v>687</v>
       </c>
@@ -11609,7 +11619,7 @@
       </c>
       <c r="G97"/>
     </row>
-    <row r="98" spans="1:7" ht="126">
+    <row r="98" spans="1:7" ht="126" hidden="1">
       <c r="A98" t="s">
         <v>957</v>
       </c>
@@ -11630,7 +11640,7 @@
       </c>
       <c r="G98"/>
     </row>
-    <row r="99" spans="1:7" ht="28">
+    <row r="99" spans="1:7" ht="28" hidden="1">
       <c r="A99" t="s">
         <v>441</v>
       </c>
@@ -11651,7 +11661,7 @@
       </c>
       <c r="G99"/>
     </row>
-    <row r="100" spans="1:7" ht="28">
+    <row r="100" spans="1:7" ht="28" hidden="1">
       <c r="A100" t="s">
         <v>669</v>
       </c>
@@ -11672,7 +11682,7 @@
       </c>
       <c r="G100"/>
     </row>
-    <row r="101" spans="1:7" ht="28">
+    <row r="101" spans="1:7" ht="28" hidden="1">
       <c r="A101" t="s">
         <v>669</v>
       </c>
@@ -11693,7 +11703,7 @@
       </c>
       <c r="G101"/>
     </row>
-    <row r="102" spans="1:7" ht="28">
+    <row r="102" spans="1:7" ht="28" hidden="1">
       <c r="A102" t="s">
         <v>687</v>
       </c>
@@ -11714,7 +11724,7 @@
       </c>
       <c r="G102"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" hidden="1">
       <c r="A103" t="s">
         <v>957</v>
       </c>
@@ -11735,7 +11745,7 @@
       </c>
       <c r="G103"/>
     </row>
-    <row r="104" spans="1:7" ht="126">
+    <row r="104" spans="1:7" ht="126" hidden="1">
       <c r="A104" t="s">
         <v>441</v>
       </c>
@@ -11756,7 +11766,7 @@
       </c>
       <c r="G104"/>
     </row>
-    <row r="105" spans="1:7" ht="28">
+    <row r="105" spans="1:7" ht="28" hidden="1">
       <c r="A105" t="s">
         <v>687</v>
       </c>
@@ -11777,7 +11787,7 @@
       </c>
       <c r="G105"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" hidden="1">
       <c r="A106" t="s">
         <v>953</v>
       </c>
@@ -11798,7 +11808,7 @@
       </c>
       <c r="G106"/>
     </row>
-    <row r="107" spans="1:7" ht="28">
+    <row r="107" spans="1:7" ht="28" hidden="1">
       <c r="A107" t="s">
         <v>687</v>
       </c>
@@ -11819,7 +11829,7 @@
       </c>
       <c r="G107"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" hidden="1">
       <c r="A108" t="s">
         <v>687</v>
       </c>
@@ -11840,7 +11850,7 @@
       </c>
       <c r="G108"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" hidden="1">
       <c r="A109" t="s">
         <v>687</v>
       </c>
@@ -11861,7 +11871,7 @@
       </c>
       <c r="G109"/>
     </row>
-    <row r="110" spans="1:7" ht="28">
+    <row r="110" spans="1:7" ht="28" hidden="1">
       <c r="A110" t="s">
         <v>968</v>
       </c>
@@ -11882,7 +11892,7 @@
       </c>
       <c r="G110"/>
     </row>
-    <row r="111" spans="1:7" ht="28">
+    <row r="111" spans="1:7" ht="28" hidden="1">
       <c r="A111" t="s">
         <v>656</v>
       </c>
@@ -11903,7 +11913,7 @@
       </c>
       <c r="G111"/>
     </row>
-    <row r="112" spans="1:7" ht="28">
+    <row r="112" spans="1:7" ht="28" hidden="1">
       <c r="A112" t="s">
         <v>758</v>
       </c>
@@ -11924,7 +11934,7 @@
       </c>
       <c r="G112"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" t="s">
         <v>450</v>
       </c>
@@ -11945,7 +11955,7 @@
       </c>
       <c r="G113"/>
     </row>
-    <row r="114" spans="1:7" ht="28">
+    <row r="114" spans="1:7" ht="28" hidden="1">
       <c r="A114" t="s">
         <v>465</v>
       </c>
@@ -11968,7 +11978,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" t="s">
         <v>478</v>
       </c>
@@ -11991,7 +12001,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" hidden="1">
       <c r="A116" t="s">
         <v>488</v>
       </c>
@@ -12012,7 +12022,7 @@
       </c>
       <c r="G116"/>
     </row>
-    <row r="117" spans="1:7" ht="28">
+    <row r="117" spans="1:7" ht="28" hidden="1">
       <c r="A117" t="s">
         <v>656</v>
       </c>
@@ -12033,7 +12043,7 @@
       </c>
       <c r="G117"/>
     </row>
-    <row r="118" spans="1:7" ht="28">
+    <row r="118" spans="1:7" ht="28" hidden="1">
       <c r="A118" t="s">
         <v>704</v>
       </c>
@@ -12054,7 +12064,7 @@
       </c>
       <c r="G118"/>
     </row>
-    <row r="119" spans="1:7" ht="28">
+    <row r="119" spans="1:7" ht="28" hidden="1">
       <c r="A119" t="s">
         <v>720</v>
       </c>
@@ -12077,7 +12087,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="28">
+    <row r="120" spans="1:7" ht="28" hidden="1">
       <c r="A120" t="s">
         <v>738</v>
       </c>
@@ -12098,7 +12108,7 @@
       </c>
       <c r="G120"/>
     </row>
-    <row r="121" spans="1:7" ht="28">
+    <row r="121" spans="1:7" ht="28" hidden="1">
       <c r="A121" t="s">
         <v>748</v>
       </c>
@@ -12119,7 +12129,7 @@
       </c>
       <c r="G121"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" t="s">
         <v>783</v>
       </c>
@@ -12140,7 +12150,7 @@
       </c>
       <c r="G122"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" t="s">
         <v>465</v>
       </c>
@@ -12161,7 +12171,7 @@
       </c>
       <c r="G123"/>
     </row>
-    <row r="124" spans="1:7" ht="28">
+    <row r="124" spans="1:7" ht="28" hidden="1">
       <c r="A124" t="s">
         <v>783</v>
       </c>
@@ -12182,7 +12192,7 @@
       </c>
       <c r="G124"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" t="s">
         <v>758</v>
       </c>
@@ -12203,7 +12213,7 @@
       </c>
       <c r="G125"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" t="s">
         <v>758</v>
       </c>
@@ -12224,7 +12234,7 @@
       </c>
       <c r="G126"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" t="s">
         <v>758</v>
       </c>
@@ -12245,7 +12255,7 @@
       </c>
       <c r="G127"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1">
       <c r="A128" t="s">
         <v>465</v>
       </c>
@@ -12266,7 +12276,7 @@
       </c>
       <c r="G128"/>
     </row>
-    <row r="129" spans="1:7" ht="98">
+    <row r="129" spans="1:7" ht="98" hidden="1">
       <c r="A129" t="s">
         <v>720</v>
       </c>
@@ -12287,7 +12297,7 @@
       </c>
       <c r="G129"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" t="s">
         <v>720</v>
       </c>
@@ -12308,7 +12318,7 @@
       </c>
       <c r="G130"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" t="s">
         <v>465</v>
       </c>
@@ -12329,7 +12339,7 @@
       </c>
       <c r="G131"/>
     </row>
-    <row r="132" spans="1:7" ht="98">
+    <row r="132" spans="1:7" ht="98" hidden="1">
       <c r="A132" t="s">
         <v>478</v>
       </c>
@@ -12350,7 +12360,7 @@
       </c>
       <c r="G132"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" t="s">
         <v>488</v>
       </c>
@@ -12371,7 +12381,7 @@
       </c>
       <c r="G133"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1">
       <c r="A134" t="s">
         <v>704</v>
       </c>
@@ -12392,7 +12402,7 @@
       </c>
       <c r="G134"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" t="s">
         <v>720</v>
       </c>
@@ -12413,7 +12423,7 @@
       </c>
       <c r="G135"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" hidden="1">
       <c r="A136" t="s">
         <v>738</v>
       </c>
@@ -12434,7 +12444,7 @@
       </c>
       <c r="G136"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1">
       <c r="A137" t="s">
         <v>748</v>
       </c>
@@ -12455,7 +12465,7 @@
       </c>
       <c r="G137"/>
     </row>
-    <row r="138" spans="1:7" ht="28">
+    <row r="138" spans="1:7" ht="28" hidden="1">
       <c r="A138" t="s">
         <v>783</v>
       </c>
@@ -12476,7 +12486,7 @@
       </c>
       <c r="G138"/>
     </row>
-    <row r="139" spans="1:7" ht="28">
+    <row r="139" spans="1:7" ht="28" hidden="1">
       <c r="A139" t="s">
         <v>720</v>
       </c>
@@ -12497,7 +12507,7 @@
       </c>
       <c r="G139"/>
     </row>
-    <row r="140" spans="1:7" ht="28">
+    <row r="140" spans="1:7" ht="28" hidden="1">
       <c r="A140" t="s">
         <v>704</v>
       </c>
@@ -12518,7 +12528,7 @@
       </c>
       <c r="G140"/>
     </row>
-    <row r="141" spans="1:7" ht="28">
+    <row r="141" spans="1:7" ht="28" hidden="1">
       <c r="A141" t="s">
         <v>465</v>
       </c>
@@ -12539,7 +12549,7 @@
       </c>
       <c r="G141"/>
     </row>
-    <row r="142" spans="1:7" ht="28">
+    <row r="142" spans="1:7" ht="28" hidden="1">
       <c r="A142" t="s">
         <v>704</v>
       </c>
@@ -12562,7 +12572,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="28">
+    <row r="143" spans="1:7" ht="28" hidden="1">
       <c r="A143" t="s">
         <v>720</v>
       </c>
@@ -12585,7 +12595,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="28">
+    <row r="144" spans="1:7" ht="28" hidden="1">
       <c r="A144" t="s">
         <v>738</v>
       </c>
@@ -12606,7 +12616,7 @@
       </c>
       <c r="G144"/>
     </row>
-    <row r="145" spans="1:7" ht="28">
+    <row r="145" spans="1:7" ht="28" hidden="1">
       <c r="A145" t="s">
         <v>738</v>
       </c>
@@ -12627,7 +12637,7 @@
       </c>
       <c r="G145"/>
     </row>
-    <row r="146" spans="1:7" ht="28">
+    <row r="146" spans="1:7" ht="28" hidden="1">
       <c r="A146" t="s">
         <v>704</v>
       </c>
@@ -12648,7 +12658,7 @@
       </c>
       <c r="G146"/>
     </row>
-    <row r="147" spans="1:7" ht="28">
+    <row r="147" spans="1:7" ht="28" hidden="1">
       <c r="A147" t="s">
         <v>748</v>
       </c>
@@ -12669,7 +12679,7 @@
       </c>
       <c r="G147"/>
     </row>
-    <row r="148" spans="1:7" ht="28">
+    <row r="148" spans="1:7" ht="28" hidden="1">
       <c r="A148" t="s">
         <v>748</v>
       </c>
@@ -12690,7 +12700,7 @@
       </c>
       <c r="G148"/>
     </row>
-    <row r="149" spans="1:7" ht="28">
+    <row r="149" spans="1:7" ht="28" hidden="1">
       <c r="A149" t="s">
         <v>783</v>
       </c>
@@ -12711,7 +12721,7 @@
       </c>
       <c r="G149"/>
     </row>
-    <row r="150" spans="1:7" ht="28">
+    <row r="150" spans="1:7" ht="28" hidden="1">
       <c r="A150" t="s">
         <v>478</v>
       </c>
@@ -12732,7 +12742,7 @@
       </c>
       <c r="G150"/>
     </row>
-    <row r="151" spans="1:7" ht="42">
+    <row r="151" spans="1:7" ht="42" hidden="1">
       <c r="A151" t="s">
         <v>488</v>
       </c>
@@ -12753,7 +12763,7 @@
       </c>
       <c r="G151"/>
     </row>
-    <row r="152" spans="1:7" ht="42">
+    <row r="152" spans="1:7" ht="42" hidden="1">
       <c r="A152" t="s">
         <v>478</v>
       </c>
@@ -12774,7 +12784,7 @@
       </c>
       <c r="G152"/>
     </row>
-    <row r="153" spans="1:7" ht="42">
+    <row r="153" spans="1:7" ht="42" hidden="1">
       <c r="A153" t="s">
         <v>488</v>
       </c>
@@ -12795,7 +12805,7 @@
       </c>
       <c r="G153"/>
     </row>
-    <row r="154" spans="1:7" ht="42">
+    <row r="154" spans="1:7" ht="42" hidden="1">
       <c r="A154" t="s">
         <v>783</v>
       </c>
@@ -12816,7 +12826,7 @@
       </c>
       <c r="G154"/>
     </row>
-    <row r="155" spans="1:7" ht="378">
+    <row r="155" spans="1:7" ht="378" hidden="1">
       <c r="A155" t="s">
         <v>488</v>
       </c>
@@ -12837,7 +12847,7 @@
       </c>
       <c r="G155"/>
     </row>
-    <row r="156" spans="1:7" ht="112">
+    <row r="156" spans="1:7" ht="112" hidden="1">
       <c r="A156" t="s">
         <v>465</v>
       </c>
@@ -12855,7 +12865,7 @@
       </c>
       <c r="G156"/>
     </row>
-    <row r="157" spans="1:7" ht="126">
+    <row r="157" spans="1:7" ht="126" hidden="1">
       <c r="A157" t="s">
         <v>720</v>
       </c>
@@ -12873,7 +12883,7 @@
       </c>
       <c r="G157"/>
     </row>
-    <row r="158" spans="1:7" ht="140">
+    <row r="158" spans="1:7" ht="140" hidden="1">
       <c r="A158" t="s">
         <v>704</v>
       </c>
@@ -12891,7 +12901,7 @@
       </c>
       <c r="G158"/>
     </row>
-    <row r="159" spans="1:7" ht="140">
+    <row r="159" spans="1:7" ht="140" hidden="1">
       <c r="A159" t="s">
         <v>720</v>
       </c>
@@ -12909,7 +12919,7 @@
       </c>
       <c r="G159"/>
     </row>
-    <row r="160" spans="1:7" ht="112">
+    <row r="160" spans="1:7" ht="112" hidden="1">
       <c r="A160" t="s">
         <v>478</v>
       </c>
@@ -12927,7 +12937,7 @@
       </c>
       <c r="G160"/>
     </row>
-    <row r="161" spans="1:7" ht="28">
+    <row r="161" spans="1:7" ht="28" hidden="1">
       <c r="A161" t="s">
         <v>704</v>
       </c>
@@ -12945,7 +12955,7 @@
       </c>
       <c r="G161"/>
     </row>
-    <row r="162" spans="1:7" ht="28">
+    <row r="162" spans="1:7" ht="28" hidden="1">
       <c r="A162" t="s">
         <v>738</v>
       </c>
@@ -12963,7 +12973,7 @@
       </c>
       <c r="G162"/>
     </row>
-    <row r="163" spans="1:7" ht="28">
+    <row r="163" spans="1:7" ht="28" hidden="1">
       <c r="A163" t="s">
         <v>748</v>
       </c>
@@ -12981,7 +12991,7 @@
       </c>
       <c r="G163"/>
     </row>
-    <row r="164" spans="1:7" ht="70">
+    <row r="164" spans="1:7" ht="70" hidden="1">
       <c r="A164" t="s">
         <v>704</v>
       </c>
@@ -12999,7 +13009,7 @@
       </c>
       <c r="G164"/>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" hidden="1">
       <c r="A165" t="s">
         <v>720</v>
       </c>
@@ -13020,7 +13030,7 @@
       </c>
       <c r="G165"/>
     </row>
-    <row r="166" spans="1:7" ht="28">
+    <row r="166" spans="1:7" ht="28" hidden="1">
       <c r="A166" t="s">
         <v>783</v>
       </c>
@@ -13054,7 +13064,7 @@
       <c r="E167" t="s">
         <v>500</v>
       </c>
-      <c r="F167" t="s">
+      <c r="F167" s="1" t="s">
         <v>1108</v>
       </c>
       <c r="G167"/>
@@ -13075,8 +13085,8 @@
       <c r="E168" t="s">
         <v>500</v>
       </c>
-      <c r="F168" t="s">
-        <v>1108</v>
+      <c r="F168" s="1" t="s">
+        <v>1110</v>
       </c>
       <c r="G168"/>
     </row>
@@ -13122,7 +13132,7 @@
       </c>
       <c r="G170"/>
     </row>
-    <row r="171" spans="1:7" ht="28">
+    <row r="171" spans="1:7" ht="42" customHeight="1">
       <c r="A171" t="s">
         <v>794</v>
       </c>
@@ -13138,8 +13148,8 @@
       <c r="E171" t="s">
         <v>500</v>
       </c>
-      <c r="F171" t="s">
-        <v>1108</v>
+      <c r="F171" s="1" t="s">
+        <v>1109</v>
       </c>
       <c r="G171"/>
     </row>
@@ -14367,7 +14377,7 @@
       </c>
       <c r="G239"/>
     </row>
-    <row r="240" spans="1:7" ht="42">
+    <row r="240" spans="1:7" ht="42" hidden="1">
       <c r="A240" t="s">
         <v>656</v>
       </c>
@@ -14385,7 +14395,7 @@
       </c>
       <c r="G240"/>
     </row>
-    <row r="241" spans="1:7" ht="42">
+    <row r="241" spans="1:7" ht="42" hidden="1">
       <c r="A241" t="s">
         <v>758</v>
       </c>
@@ -14403,7 +14413,7 @@
       </c>
       <c r="G241"/>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" hidden="1">
       <c r="A242" t="s">
         <v>886</v>
       </c>
@@ -14421,7 +14431,7 @@
       </c>
       <c r="G242"/>
     </row>
-    <row r="243" spans="1:7" ht="28">
+    <row r="243" spans="1:7" ht="28" hidden="1">
       <c r="A243" t="s">
         <v>561</v>
       </c>
@@ -14439,7 +14449,7 @@
       </c>
       <c r="G243"/>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" hidden="1">
       <c r="A244" t="s">
         <v>656</v>
       </c>
@@ -14457,7 +14467,7 @@
       </c>
       <c r="G244"/>
     </row>
-    <row r="245" spans="1:7" ht="42">
+    <row r="245" spans="1:7" ht="42" hidden="1">
       <c r="A245" t="s">
         <v>891</v>
       </c>
@@ -14475,7 +14485,7 @@
       </c>
       <c r="G245"/>
     </row>
-    <row r="246" spans="1:7" ht="28">
+    <row r="246" spans="1:7" ht="28" hidden="1">
       <c r="A246" t="s">
         <v>897</v>
       </c>
@@ -14493,7 +14503,7 @@
       </c>
       <c r="G246"/>
     </row>
-    <row r="247" spans="1:7" ht="28">
+    <row r="247" spans="1:7" ht="28" hidden="1">
       <c r="A247" t="s">
         <v>903</v>
       </c>
@@ -14511,7 +14521,7 @@
       </c>
       <c r="G247"/>
     </row>
-    <row r="248" spans="1:7" ht="98">
+    <row r="248" spans="1:7" ht="98" hidden="1">
       <c r="A248" t="s">
         <v>561</v>
       </c>
@@ -14529,7 +14539,7 @@
       </c>
       <c r="G248"/>
     </row>
-    <row r="249" spans="1:7" ht="28">
+    <row r="249" spans="1:7" ht="28" hidden="1">
       <c r="A249" t="s">
         <v>561</v>
       </c>
@@ -14547,7 +14557,7 @@
       </c>
       <c r="G249"/>
     </row>
-    <row r="250" spans="1:7" ht="28">
+    <row r="250" spans="1:7" ht="28" hidden="1">
       <c r="A250" t="s">
         <v>561</v>
       </c>
@@ -14565,7 +14575,7 @@
       </c>
       <c r="G250"/>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" hidden="1">
       <c r="A251" t="s">
         <v>758</v>
       </c>
@@ -14583,7 +14593,7 @@
       </c>
       <c r="G251"/>
     </row>
-    <row r="252" spans="1:7" ht="28">
+    <row r="252" spans="1:7" ht="28" hidden="1">
       <c r="A252" t="s">
         <v>758</v>
       </c>
@@ -14601,7 +14611,7 @@
       </c>
       <c r="G252"/>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" hidden="1">
       <c r="A253" t="s">
         <v>758</v>
       </c>
@@ -14619,7 +14629,7 @@
       </c>
       <c r="G253"/>
     </row>
-    <row r="254" spans="1:7" ht="56">
+    <row r="254" spans="1:7" ht="56" hidden="1">
       <c r="A254" t="s">
         <v>561</v>
       </c>
@@ -14637,7 +14647,7 @@
       </c>
       <c r="G254"/>
     </row>
-    <row r="255" spans="1:7" ht="28">
+    <row r="255" spans="1:7" ht="28" hidden="1">
       <c r="A255" t="s">
         <v>561</v>
       </c>
@@ -14655,7 +14665,7 @@
       </c>
       <c r="G255"/>
     </row>
-    <row r="256" spans="1:7" ht="42">
+    <row r="256" spans="1:7" ht="42" hidden="1">
       <c r="A256" t="s">
         <v>561</v>
       </c>
@@ -14673,7 +14683,7 @@
       </c>
       <c r="G256"/>
     </row>
-    <row r="257" spans="1:7" ht="28">
+    <row r="257" spans="1:7" ht="28" hidden="1">
       <c r="A257" t="s">
         <v>891</v>
       </c>
@@ -14691,7 +14701,7 @@
       </c>
       <c r="G257"/>
     </row>
-    <row r="258" spans="1:7" ht="28">
+    <row r="258" spans="1:7" ht="28" hidden="1">
       <c r="A258" t="s">
         <v>897</v>
       </c>
@@ -14709,7 +14719,7 @@
       </c>
       <c r="G258"/>
     </row>
-    <row r="259" spans="1:7" ht="28">
+    <row r="259" spans="1:7" ht="28" hidden="1">
       <c r="A259" t="s">
         <v>903</v>
       </c>
@@ -14727,7 +14737,7 @@
       </c>
       <c r="G259"/>
     </row>
-    <row r="260" spans="1:7" ht="28">
+    <row r="260" spans="1:7" ht="28" hidden="1">
       <c r="A260" t="s">
         <v>891</v>
       </c>
@@ -14745,7 +14755,7 @@
       </c>
       <c r="G260"/>
     </row>
-    <row r="261" spans="1:7" ht="266">
+    <row r="261" spans="1:7" ht="266" hidden="1">
       <c r="A261" t="s">
         <v>561</v>
       </c>
@@ -14763,7 +14773,7 @@
       </c>
       <c r="G261"/>
     </row>
-    <row r="262" spans="1:7" ht="42">
+    <row r="262" spans="1:7" ht="42" hidden="1">
       <c r="A262" t="s">
         <v>561</v>
       </c>
@@ -14781,7 +14791,7 @@
       </c>
       <c r="G262"/>
     </row>
-    <row r="263" spans="1:7" ht="42">
+    <row r="263" spans="1:7" ht="42" hidden="1">
       <c r="A263" t="s">
         <v>886</v>
       </c>
@@ -14799,7 +14809,7 @@
       </c>
       <c r="G263"/>
     </row>
-    <row r="264" spans="1:7" ht="28">
+    <row r="264" spans="1:7" ht="28" hidden="1">
       <c r="A264" t="s">
         <v>897</v>
       </c>
@@ -14817,7 +14827,7 @@
       </c>
       <c r="G264"/>
     </row>
-    <row r="265" spans="1:7" ht="28">
+    <row r="265" spans="1:7" ht="28" hidden="1">
       <c r="A265" t="s">
         <v>582</v>
       </c>
@@ -14835,7 +14845,7 @@
       </c>
       <c r="G265"/>
     </row>
-    <row r="266" spans="1:7" ht="28">
+    <row r="266" spans="1:7" ht="28" hidden="1">
       <c r="A266" t="s">
         <v>588</v>
       </c>
@@ -14853,7 +14863,7 @@
       </c>
       <c r="G266"/>
     </row>
-    <row r="267" spans="1:7" ht="28">
+    <row r="267" spans="1:7" ht="28" hidden="1">
       <c r="A267" t="s">
         <v>600</v>
       </c>
@@ -14871,7 +14881,7 @@
       </c>
       <c r="G267"/>
     </row>
-    <row r="268" spans="1:7" ht="28">
+    <row r="268" spans="1:7" ht="28" hidden="1">
       <c r="A268" t="s">
         <v>603</v>
       </c>
@@ -14889,7 +14899,7 @@
       </c>
       <c r="G268"/>
     </row>
-    <row r="269" spans="1:7" ht="42">
+    <row r="269" spans="1:7" ht="42" hidden="1">
       <c r="A269" t="s">
         <v>606</v>
       </c>
@@ -14907,7 +14917,7 @@
       </c>
       <c r="G269"/>
     </row>
-    <row r="270" spans="1:7" ht="28">
+    <row r="270" spans="1:7" ht="28" hidden="1">
       <c r="A270" t="s">
         <v>613</v>
       </c>
@@ -14925,7 +14935,7 @@
       </c>
       <c r="G270"/>
     </row>
-    <row r="271" spans="1:7" ht="42">
+    <row r="271" spans="1:7" ht="42" hidden="1">
       <c r="A271" t="s">
         <v>630</v>
       </c>
@@ -14943,7 +14953,7 @@
       </c>
       <c r="G271"/>
     </row>
-    <row r="272" spans="1:7" ht="112">
+    <row r="272" spans="1:7" ht="112" hidden="1">
       <c r="A272" t="s">
         <v>650</v>
       </c>
@@ -14961,7 +14971,7 @@
       </c>
       <c r="G272"/>
     </row>
-    <row r="273" spans="1:7" ht="28">
+    <row r="273" spans="1:7" ht="28" hidden="1">
       <c r="A273" t="s">
         <v>656</v>
       </c>
@@ -14979,7 +14989,7 @@
       </c>
       <c r="G273"/>
     </row>
-    <row r="274" spans="1:7" ht="28">
+    <row r="274" spans="1:7" ht="28" hidden="1">
       <c r="A274" t="s">
         <v>758</v>
       </c>
@@ -14997,7 +15007,7 @@
       </c>
       <c r="G274"/>
     </row>
-    <row r="275" spans="1:7" ht="42">
+    <row r="275" spans="1:7" ht="42" hidden="1">
       <c r="A275" t="s">
         <v>913</v>
       </c>
@@ -15015,7 +15025,7 @@
       </c>
       <c r="G275"/>
     </row>
-    <row r="276" spans="1:7" ht="28">
+    <row r="276" spans="1:7" ht="28" hidden="1">
       <c r="A276" t="s">
         <v>924</v>
       </c>
@@ -15033,7 +15043,7 @@
       </c>
       <c r="G276"/>
     </row>
-    <row r="277" spans="1:7" ht="28">
+    <row r="277" spans="1:7" ht="28" hidden="1">
       <c r="A277" t="s">
         <v>432</v>
       </c>
@@ -15051,7 +15061,7 @@
       </c>
       <c r="G277"/>
     </row>
-    <row r="278" spans="1:7" ht="28">
+    <row r="278" spans="1:7" ht="28" hidden="1">
       <c r="A278" t="s">
         <v>438</v>
       </c>
@@ -15069,7 +15079,7 @@
       </c>
       <c r="G278"/>
     </row>
-    <row r="279" spans="1:7" ht="28">
+    <row r="279" spans="1:7" ht="28" hidden="1">
       <c r="A279" t="s">
         <v>613</v>
       </c>
@@ -15087,7 +15097,7 @@
       </c>
       <c r="G279"/>
     </row>
-    <row r="280" spans="1:7" ht="42">
+    <row r="280" spans="1:7" ht="42" hidden="1">
       <c r="A280" t="s">
         <v>653</v>
       </c>
@@ -15105,7 +15115,7 @@
       </c>
       <c r="G280"/>
     </row>
-    <row r="281" spans="1:7" ht="28">
+    <row r="281" spans="1:7" ht="28" hidden="1">
       <c r="A281" t="s">
         <v>656</v>
       </c>
@@ -15123,7 +15133,7 @@
       </c>
       <c r="G281"/>
     </row>
-    <row r="282" spans="1:7" ht="98">
+    <row r="282" spans="1:7" ht="98" hidden="1">
       <c r="A282" t="s">
         <v>938</v>
       </c>
@@ -15141,7 +15151,7 @@
       </c>
       <c r="G282"/>
     </row>
-    <row r="283" spans="1:7" ht="56">
+    <row r="283" spans="1:7" ht="56" hidden="1">
       <c r="A283" t="s">
         <v>941</v>
       </c>
@@ -15159,7 +15169,7 @@
       </c>
       <c r="G283"/>
     </row>
-    <row r="284" spans="1:7" ht="70">
+    <row r="284" spans="1:7" ht="70" hidden="1">
       <c r="A284" t="s">
         <v>913</v>
       </c>
@@ -15177,7 +15187,7 @@
       </c>
       <c r="G284"/>
     </row>
-    <row r="285" spans="1:7" ht="28">
+    <row r="285" spans="1:7" ht="28" hidden="1">
       <c r="A285" t="s">
         <v>613</v>
       </c>
@@ -15195,7 +15205,7 @@
       </c>
       <c r="G285"/>
     </row>
-    <row r="286" spans="1:7" ht="98">
+    <row r="286" spans="1:7" ht="98" hidden="1">
       <c r="A286" t="s">
         <v>613</v>
       </c>
@@ -15213,7 +15223,7 @@
       </c>
       <c r="G286"/>
     </row>
-    <row r="287" spans="1:7" ht="56">
+    <row r="287" spans="1:7" ht="56" hidden="1">
       <c r="A287" t="s">
         <v>630</v>
       </c>
@@ -15231,7 +15241,7 @@
       </c>
       <c r="G287"/>
     </row>
-    <row r="288" spans="1:7" ht="28">
+    <row r="288" spans="1:7" ht="28" hidden="1">
       <c r="A288" t="s">
         <v>630</v>
       </c>
@@ -15249,7 +15259,7 @@
       </c>
       <c r="G288"/>
     </row>
-    <row r="289" spans="1:7" ht="28">
+    <row r="289" spans="1:7" ht="28" hidden="1">
       <c r="A289" t="s">
         <v>630</v>
       </c>
@@ -15267,7 +15277,7 @@
       </c>
       <c r="G289"/>
     </row>
-    <row r="290" spans="1:7" ht="28">
+    <row r="290" spans="1:7" ht="28" hidden="1">
       <c r="A290" t="s">
         <v>588</v>
       </c>
@@ -15285,7 +15295,7 @@
       </c>
       <c r="G290"/>
     </row>
-    <row r="291" spans="1:7" ht="28">
+    <row r="291" spans="1:7" ht="28" hidden="1">
       <c r="A291" t="s">
         <v>758</v>
       </c>
@@ -15303,7 +15313,7 @@
       </c>
       <c r="G291"/>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:7" hidden="1">
       <c r="A292" t="s">
         <v>588</v>
       </c>
@@ -15321,7 +15331,7 @@
       </c>
       <c r="G292"/>
     </row>
-    <row r="293" spans="1:7" ht="56">
+    <row r="293" spans="1:7" ht="56" hidden="1">
       <c r="A293" t="s">
         <v>758</v>
       </c>
@@ -15339,7 +15349,7 @@
       </c>
       <c r="G293"/>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" hidden="1">
       <c r="A294" t="s">
         <v>588</v>
       </c>
@@ -15357,7 +15367,7 @@
       </c>
       <c r="G294"/>
     </row>
-    <row r="295" spans="1:7" ht="28">
+    <row r="295" spans="1:7" ht="28" hidden="1">
       <c r="A295" t="s">
         <v>758</v>
       </c>
@@ -15375,7 +15385,7 @@
       </c>
       <c r="G295"/>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:7" hidden="1">
       <c r="A296" t="s">
         <v>913</v>
       </c>
@@ -15393,7 +15403,7 @@
       </c>
       <c r="G296"/>
     </row>
-    <row r="297" spans="1:7" ht="28">
+    <row r="297" spans="1:7" ht="28" hidden="1">
       <c r="A297" t="s">
         <v>630</v>
       </c>
@@ -15411,7 +15421,7 @@
       </c>
       <c r="G297"/>
     </row>
-    <row r="298" spans="1:7" ht="28">
+    <row r="298" spans="1:7" ht="28" hidden="1">
       <c r="A298" t="s">
         <v>432</v>
       </c>
@@ -15429,7 +15439,7 @@
       </c>
       <c r="G298"/>
     </row>
-    <row r="299" spans="1:7" ht="28">
+    <row r="299" spans="1:7" ht="28" hidden="1">
       <c r="A299" t="s">
         <v>438</v>
       </c>
@@ -15447,7 +15457,7 @@
       </c>
       <c r="G299"/>
     </row>
-    <row r="300" spans="1:7" ht="84">
+    <row r="300" spans="1:7" ht="84" hidden="1">
       <c r="A300" t="s">
         <v>941</v>
       </c>
@@ -15465,7 +15475,7 @@
       </c>
       <c r="G300"/>
     </row>
-    <row r="301" spans="1:7" ht="42">
+    <row r="301" spans="1:7" ht="42" hidden="1">
       <c r="A301" t="s">
         <v>630</v>
       </c>
@@ -15483,7 +15493,7 @@
       </c>
       <c r="G301"/>
     </row>
-    <row r="302" spans="1:7" ht="28">
+    <row r="302" spans="1:7" ht="28" hidden="1">
       <c r="A302" t="s">
         <v>941</v>
       </c>
@@ -15501,7 +15511,7 @@
       </c>
       <c r="G302"/>
     </row>
-    <row r="303" spans="1:7" ht="28">
+    <row r="303" spans="1:7" ht="28" hidden="1">
       <c r="A303" t="s">
         <v>941</v>
       </c>
@@ -15519,7 +15529,7 @@
       </c>
       <c r="G303"/>
     </row>
-    <row r="304" spans="1:7" ht="84">
+    <row r="304" spans="1:7" ht="84" hidden="1">
       <c r="A304" t="s">
         <v>613</v>
       </c>
@@ -15537,7 +15547,7 @@
       </c>
       <c r="G304"/>
     </row>
-    <row r="305" spans="1:7" ht="42">
+    <row r="305" spans="1:7" ht="42" hidden="1">
       <c r="A305" t="s">
         <v>613</v>
       </c>
@@ -15555,7 +15565,7 @@
       </c>
       <c r="G305"/>
     </row>
-    <row r="306" spans="1:7" ht="28">
+    <row r="306" spans="1:7" ht="28" hidden="1">
       <c r="A306" t="s">
         <v>913</v>
       </c>
@@ -15573,7 +15583,7 @@
       </c>
       <c r="G306"/>
     </row>
-    <row r="307" spans="1:7" ht="154">
+    <row r="307" spans="1:7" ht="154" hidden="1">
       <c r="A307" t="s">
         <v>924</v>
       </c>
@@ -15591,7 +15601,7 @@
       </c>
       <c r="G307"/>
     </row>
-    <row r="308" spans="1:7" ht="238">
+    <row r="308" spans="1:7" ht="238" hidden="1">
       <c r="A308" t="s">
         <v>432</v>
       </c>
@@ -15609,7 +15619,7 @@
       </c>
       <c r="G308"/>
     </row>
-    <row r="309" spans="1:7" ht="28">
+    <row r="309" spans="1:7" ht="28" hidden="1">
       <c r="A309" t="s">
         <v>606</v>
       </c>
@@ -15627,7 +15637,7 @@
       </c>
       <c r="G309"/>
     </row>
-    <row r="310" spans="1:7" ht="28">
+    <row r="310" spans="1:7" ht="28" hidden="1">
       <c r="A310" t="s">
         <v>438</v>
       </c>
@@ -15645,7 +15655,7 @@
       </c>
       <c r="G310"/>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" hidden="1">
       <c r="A311" t="s">
         <v>582</v>
       </c>
@@ -15663,7 +15673,7 @@
       </c>
       <c r="G311"/>
     </row>
-    <row r="312" spans="1:7" ht="28">
+    <row r="312" spans="1:7" ht="28" hidden="1">
       <c r="A312" t="s">
         <v>588</v>
       </c>
@@ -15681,7 +15691,7 @@
       </c>
       <c r="G312"/>
     </row>
-    <row r="313" spans="1:7" ht="28">
+    <row r="313" spans="1:7" ht="28" hidden="1">
       <c r="A313" t="s">
         <v>600</v>
       </c>
@@ -15699,7 +15709,7 @@
       </c>
       <c r="G313"/>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:7" hidden="1">
       <c r="A314" t="s">
         <v>606</v>
       </c>
@@ -15717,7 +15727,7 @@
       </c>
       <c r="G314"/>
     </row>
-    <row r="315" spans="1:7" ht="42">
+    <row r="315" spans="1:7" ht="42" hidden="1">
       <c r="A315" t="s">
         <v>613</v>
       </c>
@@ -15735,7 +15745,7 @@
       </c>
       <c r="G315"/>
     </row>
-    <row r="316" spans="1:7" ht="126">
+    <row r="316" spans="1:7" ht="126" hidden="1">
       <c r="A316" t="s">
         <v>630</v>
       </c>
@@ -15753,7 +15763,7 @@
       </c>
       <c r="G316"/>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" hidden="1">
       <c r="A317" t="s">
         <v>650</v>
       </c>
@@ -15771,7 +15781,7 @@
       </c>
       <c r="G317"/>
     </row>
-    <row r="318" spans="1:7" ht="56">
+    <row r="318" spans="1:7" ht="56" hidden="1">
       <c r="A318" t="s">
         <v>913</v>
       </c>
@@ -15789,7 +15799,7 @@
       </c>
       <c r="G318"/>
     </row>
-    <row r="319" spans="1:7" ht="28">
+    <row r="319" spans="1:7" ht="28" hidden="1">
       <c r="A319" t="s">
         <v>924</v>
       </c>
@@ -15807,7 +15817,7 @@
       </c>
       <c r="G319"/>
     </row>
-    <row r="320" spans="1:7" ht="28">
+    <row r="320" spans="1:7" ht="28" hidden="1">
       <c r="A320" t="s">
         <v>613</v>
       </c>
@@ -15825,7 +15835,7 @@
       </c>
       <c r="G320"/>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:7" hidden="1">
       <c r="A321" t="s">
         <v>653</v>
       </c>
@@ -15843,7 +15853,7 @@
       </c>
       <c r="G321"/>
     </row>
-    <row r="322" spans="1:7">
+    <row r="322" spans="1:7" hidden="1">
       <c r="A322" t="s">
         <v>938</v>
       </c>
@@ -15861,7 +15871,7 @@
       </c>
       <c r="G322"/>
     </row>
-    <row r="323" spans="1:7" ht="28">
+    <row r="323" spans="1:7" ht="28" hidden="1">
       <c r="A323" t="s">
         <v>941</v>
       </c>
@@ -15879,7 +15889,7 @@
       </c>
       <c r="G323"/>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" hidden="1">
       <c r="A324" t="s">
         <v>1043</v>
       </c>
@@ -15897,7 +15907,7 @@
       </c>
       <c r="G324"/>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:7" hidden="1">
       <c r="A325" t="s">
         <v>1041</v>
       </c>
@@ -15915,7 +15925,7 @@
       </c>
       <c r="G325"/>
     </row>
-    <row r="326" spans="1:7">
+    <row r="326" spans="1:7" hidden="1">
       <c r="A326" t="s">
         <v>913</v>
       </c>
@@ -15933,7 +15943,7 @@
       </c>
       <c r="G326"/>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:7" hidden="1">
       <c r="A327" t="s">
         <v>613</v>
       </c>
@@ -15951,7 +15961,7 @@
       </c>
       <c r="G327"/>
     </row>
-    <row r="328" spans="1:7">
+    <row r="328" spans="1:7" hidden="1">
       <c r="A328" t="s">
         <v>613</v>
       </c>
@@ -15969,7 +15979,7 @@
       </c>
       <c r="G328"/>
     </row>
-    <row r="329" spans="1:7">
+    <row r="329" spans="1:7" hidden="1">
       <c r="A329" t="s">
         <v>630</v>
       </c>
@@ -15987,7 +15997,7 @@
       </c>
       <c r="G329"/>
     </row>
-    <row r="330" spans="1:7" ht="56">
+    <row r="330" spans="1:7" ht="56" hidden="1">
       <c r="A330" t="s">
         <v>630</v>
       </c>
@@ -16005,7 +16015,7 @@
       </c>
       <c r="G330"/>
     </row>
-    <row r="331" spans="1:7">
+    <row r="331" spans="1:7" hidden="1">
       <c r="A331" t="s">
         <v>630</v>
       </c>
@@ -16023,7 +16033,7 @@
       </c>
       <c r="G331"/>
     </row>
-    <row r="332" spans="1:7">
+    <row r="332" spans="1:7" hidden="1">
       <c r="A332" t="s">
         <v>588</v>
       </c>
@@ -16041,7 +16051,7 @@
       </c>
       <c r="G332"/>
     </row>
-    <row r="333" spans="1:7">
+    <row r="333" spans="1:7" hidden="1">
       <c r="A333" t="s">
         <v>588</v>
       </c>
@@ -16059,7 +16069,7 @@
       </c>
       <c r="G333"/>
     </row>
-    <row r="334" spans="1:7">
+    <row r="334" spans="1:7" hidden="1">
       <c r="A334" t="s">
         <v>588</v>
       </c>
@@ -16077,7 +16087,7 @@
       </c>
       <c r="G334"/>
     </row>
-    <row r="335" spans="1:7">
+    <row r="335" spans="1:7" hidden="1">
       <c r="A335" t="s">
         <v>913</v>
       </c>
@@ -16095,7 +16105,7 @@
       </c>
       <c r="G335"/>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" hidden="1">
       <c r="A336" t="s">
         <v>630</v>
       </c>
@@ -16113,7 +16123,7 @@
       </c>
       <c r="G336"/>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1">
       <c r="A337" t="s">
         <v>941</v>
       </c>
@@ -16131,7 +16141,7 @@
       </c>
       <c r="G337"/>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" hidden="1">
       <c r="A338" t="s">
         <v>630</v>
       </c>
@@ -16149,7 +16159,7 @@
       </c>
       <c r="G338"/>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" t="s">
         <v>941</v>
       </c>
@@ -16167,7 +16177,7 @@
       </c>
       <c r="G339"/>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" t="s">
         <v>941</v>
       </c>
@@ -16185,7 +16195,7 @@
       </c>
       <c r="G340"/>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" t="s">
         <v>613</v>
       </c>
@@ -16203,7 +16213,7 @@
       </c>
       <c r="G341"/>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" t="s">
         <v>613</v>
       </c>
@@ -16221,7 +16231,7 @@
       </c>
       <c r="G342"/>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" t="s">
         <v>924</v>
       </c>
@@ -16239,7 +16249,7 @@
       </c>
       <c r="G343"/>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" t="s">
         <v>606</v>
       </c>
@@ -16257,7 +16267,7 @@
       </c>
       <c r="G344"/>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" t="s">
         <v>630</v>
       </c>
@@ -16277,6 +16287,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G345">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:G345">
       <sortCondition ref="C1:C345"/>
     </sortState>

</xml_diff>

<commit_message>
updated spreadsheet for victim test
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="1112">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -4987,6 +4987,10 @@
   <si>
     <t>0a2055d
 facbory test: 56069d2</t>
+  </si>
+  <si>
+    <t>factory test: ba41427
+todo: account for it being optional</t>
   </si>
 </sst>
 </file>
@@ -9685,7 +9689,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167:F171"/>
+      <selection activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9695,7 +9699,7 @@
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13186,6 +13190,9 @@
       </c>
       <c r="E173" t="s">
         <v>500</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>1111</v>
       </c>
       <c r="G173"/>
     </row>

</xml_diff>

<commit_message>
updated nibrs spreadsheet for validation rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="1113">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -4991,6 +4991,9 @@
   <si>
     <t>factory test: ba41427
 todo: account for it being optional</t>
+  </si>
+  <si>
+    <t>factory test: 635c756</t>
   </si>
 </sst>
 </file>
@@ -9689,7 +9692,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F174" sqref="F174"/>
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13211,6 +13214,9 @@
       </c>
       <c r="E174" t="s">
         <v>500</v>
+      </c>
+      <c r="F174" t="s">
+        <v>1112</v>
       </c>
       <c r="G174"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for unit test added
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="1114">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -4994,6 +4994,9 @@
   </si>
   <si>
     <t>factory test: 635c756</t>
+  </si>
+  <si>
+    <t>factory test: d6eda9f</t>
   </si>
 </sst>
 </file>
@@ -9692,7 +9695,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E174" sqref="E174"/>
+      <selection activeCell="F175" sqref="A175:F175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13220,7 +13223,7 @@
       </c>
       <c r="G174"/>
     </row>
-    <row r="175" spans="1:7" ht="42">
+    <row r="175" spans="1:7" ht="28">
       <c r="A175" t="s">
         <v>536</v>
       </c>
@@ -13235,6 +13238,9 @@
       </c>
       <c r="E175" t="s">
         <v>500</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>1113</v>
       </c>
       <c r="G175"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with unit test added: testRule404ForTypeOfficerActivityCircumstance()
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="1116">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5000,6 +5000,9 @@
   </si>
   <si>
     <t>factory test:  92ef219</t>
+  </si>
+  <si>
+    <t>factory test:  7fc6b93</t>
   </si>
 </sst>
 </file>
@@ -9698,7 +9701,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F176" sqref="F176"/>
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13284,6 +13287,9 @@
       <c r="E177" t="s">
         <v>500</v>
       </c>
+      <c r="F177" s="1" t="s">
+        <v>984</v>
+      </c>
       <c r="G177"/>
     </row>
     <row r="178" spans="1:7" ht="28">
@@ -13301,6 +13307,9 @@
       </c>
       <c r="E178" t="s">
         <v>500</v>
+      </c>
+      <c r="F178" t="s">
+        <v>1115</v>
       </c>
       <c r="G178"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new unit test added
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="1117">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5003,6 +5003,9 @@
   </si>
   <si>
     <t>factory test:  7fc6b93</t>
+  </si>
+  <si>
+    <t>factory test:  e006bfa39839e3f98510a56b2bc93d44ed2a43a9</t>
   </si>
 </sst>
 </file>
@@ -9701,7 +9704,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9711,7 +9714,7 @@
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13328,6 +13331,9 @@
       </c>
       <c r="E179" t="s">
         <v>500</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>1116</v>
       </c>
       <c r="G179"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new ori rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="1118">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5006,6 +5006,9 @@
   </si>
   <si>
     <t>factory test:  e006bfa39839e3f98510a56b2bc93d44ed2a43a9</t>
+  </si>
+  <si>
+    <t>factory test:  b05a4e9f96db70f49ff236da8d6988e2f275a20e</t>
   </si>
 </sst>
 </file>
@@ -9704,7 +9707,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13352,6 +13355,9 @@
       </c>
       <c r="E180" t="s">
         <v>500</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1117</v>
       </c>
       <c r="G180"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new validatoin factory rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2925" uniqueCount="1119">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5005,10 +5005,13 @@
     <t>factory test:  7fc6b93</t>
   </si>
   <si>
-    <t>factory test:  e006bfa39839e3f98510a56b2bc93d44ed2a43a9</t>
-  </si>
-  <si>
-    <t>factory test:  b05a4e9f96db70f49ff236da8d6988e2f275a20e</t>
+    <t>factory test:  aa2c92c</t>
+  </si>
+  <si>
+    <t>factory test:  b05a4e9</t>
+  </si>
+  <si>
+    <t>factory test:  e006bfa</t>
   </si>
 </sst>
 </file>
@@ -9707,7 +9710,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D181" sqref="D181"/>
+      <selection activeCell="F182" sqref="C182:F182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13336,7 +13339,7 @@
         <v>500</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="G179"/>
     </row>
@@ -13376,6 +13379,9 @@
       </c>
       <c r="E181" t="s">
         <v>500</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>1116</v>
       </c>
       <c r="G181"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new validation rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2925" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="1121">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5012,6 +5012,12 @@
   </si>
   <si>
     <t>factory test:  e006bfa</t>
+  </si>
+  <si>
+    <t>factory test:  d4e4f1e</t>
+  </si>
+  <si>
+    <t>factory test:  ddda579</t>
   </si>
 </sst>
 </file>
@@ -9710,7 +9716,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F182" sqref="C182:F182"/>
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13401,6 +13407,9 @@
       <c r="E182" t="s">
         <v>500</v>
       </c>
+      <c r="F182" t="s">
+        <v>1119</v>
+      </c>
       <c r="G182"/>
     </row>
     <row r="183" spans="1:7" ht="28">
@@ -13418,6 +13427,9 @@
       </c>
       <c r="E183" t="s">
         <v>500</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>1120</v>
       </c>
       <c r="G183"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for validation test
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="1122">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5018,6 +5018,9 @@
   </si>
   <si>
     <t>factory test:  ddda579</t>
+  </si>
+  <si>
+    <t>factory test: e7915b9</t>
   </si>
 </sst>
 </file>
@@ -9716,7 +9719,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F183" sqref="F183"/>
+      <selection activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13448,6 +13451,9 @@
       </c>
       <c r="E184" t="s">
         <v>500</v>
+      </c>
+      <c r="F184" t="s">
+        <v>1121</v>
       </c>
       <c r="G184"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new victim rule unit test
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="1124">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5021,6 +5021,12 @@
   </si>
   <si>
     <t>factory test: e7915b9</t>
+  </si>
+  <si>
+    <t>factory test:  d6c28e2</t>
+  </si>
+  <si>
+    <t>factory test:  8b6dd95</t>
   </si>
 </sst>
 </file>
@@ -9719,7 +9725,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F185" sqref="F185"/>
+      <selection activeCell="F187" sqref="C187:F187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13473,6 +13479,9 @@
       <c r="E185" t="s">
         <v>500</v>
       </c>
+      <c r="F185" s="1" t="s">
+        <v>1122</v>
+      </c>
       <c r="G185"/>
     </row>
     <row r="186" spans="1:7" ht="28">
@@ -13490,6 +13499,9 @@
       </c>
       <c r="E186" t="s">
         <v>500</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1123</v>
       </c>
       <c r="G186"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with validation rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2931" uniqueCount="1125">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5027,6 +5027,9 @@
   </si>
   <si>
     <t>factory test:  8b6dd95</t>
+  </si>
+  <si>
+    <t>factory test:  26ae22a</t>
   </si>
 </sst>
 </file>
@@ -9724,8 +9727,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F187" sqref="C187:F187"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="F188" sqref="D188:F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13520,6 +13523,9 @@
       </c>
       <c r="E187" t="s">
         <v>500</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>1124</v>
       </c>
       <c r="G187"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for duplicate injury rule just added
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2931" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2933" uniqueCount="1127">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5030,6 +5030,12 @@
   </si>
   <si>
     <t>factory test:  26ae22a</t>
+  </si>
+  <si>
+    <t>factory test: 610f4b</t>
+  </si>
+  <si>
+    <t>factory test: d975140</t>
   </si>
 </sst>
 </file>
@@ -9728,7 +9734,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="F188" sqref="D188:F188"/>
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13545,6 +13551,9 @@
       <c r="E188" t="s">
         <v>500</v>
       </c>
+      <c r="F188" t="s">
+        <v>1125</v>
+      </c>
       <c r="G188"/>
     </row>
     <row r="189" spans="1:7" ht="28">
@@ -13562,6 +13571,9 @@
       </c>
       <c r="E189" t="s">
         <v>500</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>1126</v>
       </c>
       <c r="G189"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for validation rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2933" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2934" uniqueCount="1128">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5036,6 +5036,9 @@
   </si>
   <si>
     <t>factory test: d975140</t>
+  </si>
+  <si>
+    <t>factory test:  f53e20a</t>
   </si>
 </sst>
 </file>
@@ -9733,8 +9736,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="F190" sqref="F190"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13217,6 +13220,9 @@
       </c>
       <c r="E172" t="s">
         <v>500</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>1127</v>
       </c>
       <c r="G172"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with new age range rule added
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2934" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2940" uniqueCount="1131">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5039,6 +5039,15 @@
   </si>
   <si>
     <t>factory test:  f53e20a</t>
+  </si>
+  <si>
+    <t>N/A - handled by flat file importer</t>
+  </si>
+  <si>
+    <t>factory test:  38dfa33</t>
+  </si>
+  <si>
+    <t>N/A - handled by admin segment</t>
   </si>
 </sst>
 </file>
@@ -9736,17 +9745,17 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+    <sheetView tabSelected="1" topLeftCell="B183" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
     <col min="4" max="4" width="100.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
     <col min="6" max="6" width="50.6640625" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
   </cols>
@@ -13617,6 +13626,9 @@
       <c r="E191" t="s">
         <v>500</v>
       </c>
+      <c r="F191" s="1" t="s">
+        <v>1128</v>
+      </c>
       <c r="G191"/>
     </row>
     <row r="192" spans="1:7" ht="28">
@@ -13635,6 +13647,9 @@
       <c r="E192" t="s">
         <v>500</v>
       </c>
+      <c r="F192" t="s">
+        <v>1128</v>
+      </c>
       <c r="G192"/>
     </row>
     <row r="193" spans="1:7">
@@ -13653,6 +13668,9 @@
       <c r="E193" t="s">
         <v>500</v>
       </c>
+      <c r="F193" s="1" t="s">
+        <v>1129</v>
+      </c>
       <c r="G193"/>
     </row>
     <row r="194" spans="1:7" ht="28">
@@ -13671,6 +13689,9 @@
       <c r="E194" t="s">
         <v>500</v>
       </c>
+      <c r="F194" t="s">
+        <v>1130</v>
+      </c>
       <c r="G194"/>
     </row>
     <row r="195" spans="1:7">
@@ -13689,6 +13710,9 @@
       <c r="E195" t="s">
         <v>500</v>
       </c>
+      <c r="F195" s="1" t="s">
+        <v>1130</v>
+      </c>
       <c r="G195"/>
     </row>
     <row r="196" spans="1:7" ht="70">
@@ -13706,6 +13730,9 @@
       </c>
       <c r="E196" t="s">
         <v>500</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1130</v>
       </c>
       <c r="G196"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new factory test rule
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2940" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1132">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5048,6 +5048,9 @@
   </si>
   <si>
     <t>N/A - handled by admin segment</t>
+  </si>
+  <si>
+    <t>testRule419ForAggravatedAssaultHomicideCircumstances</t>
   </si>
 </sst>
 </file>
@@ -9745,8 +9748,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B183" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F183" sqref="F183"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E197" sqref="E197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13751,6 +13754,9 @@
       </c>
       <c r="E197" t="s">
         <v>500</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1131</v>
       </c>
       <c r="G197"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with new victim rule factory test
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="1133">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5051,6 +5051,9 @@
   </si>
   <si>
     <t>testRule419ForAggravatedAssaultHomicideCircumstances</t>
+  </si>
+  <si>
+    <t>aae8824</t>
   </si>
 </sst>
 </file>
@@ -9748,8 +9751,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E197" sqref="E197"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="E199" sqref="E199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9759,7 +9762,7 @@
     <col min="3" max="3" width="7.83203125" customWidth="1"/>
     <col min="4" max="4" width="100.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13793,6 +13796,9 @@
       </c>
       <c r="E199" t="s">
         <v>500</v>
+      </c>
+      <c r="F199" t="s">
+        <v>1132</v>
       </c>
       <c r="G199"/>
     </row>

</xml_diff>

<commit_message>
updated rules spreadsheet for new factory test: testRule450ForAgeOfVictim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="1134">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5054,6 +5054,9 @@
   </si>
   <si>
     <t>aae8824</t>
+  </si>
+  <si>
+    <t>b439de0</t>
   </si>
 </sst>
 </file>
@@ -9751,8 +9754,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="E199" sqref="E199"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="F201" sqref="F201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13817,6 +13820,9 @@
       </c>
       <c r="E200" t="s">
         <v>500</v>
+      </c>
+      <c r="F200" t="s">
+        <v>1133</v>
       </c>
       <c r="G200"/>
     </row>

</xml_diff>

<commit_message>
edited rule spreadsheet, added test: testRule453ForAgeOfVictim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="1135">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5057,6 +5057,9 @@
   </si>
   <si>
     <t>b439de0</t>
+  </si>
+  <si>
+    <t>b1b8584</t>
   </si>
 </sst>
 </file>
@@ -9755,7 +9758,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="F201" sqref="F201"/>
+      <selection activeCell="C202" sqref="C202:E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13841,6 +13844,9 @@
       </c>
       <c r="E201" t="s">
         <v>500</v>
+      </c>
+      <c r="F201" t="s">
+        <v>1134</v>
       </c>
       <c r="G201"/>
     </row>

</xml_diff>

<commit_message>
edited rules spreadsheet, added rule: testRule453ForRaceOfVictim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="1137">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5060,6 +5060,12 @@
   </si>
   <si>
     <t>b1b8584</t>
+  </si>
+  <si>
+    <t>5bb1136</t>
+  </si>
+  <si>
+    <t>bdac265</t>
   </si>
 </sst>
 </file>
@@ -9758,7 +9764,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="C202" sqref="C202:E202"/>
+      <selection activeCell="D203" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13866,6 +13872,9 @@
       <c r="E202" t="s">
         <v>500</v>
       </c>
+      <c r="F202" t="s">
+        <v>1135</v>
+      </c>
       <c r="G202"/>
     </row>
     <row r="203" spans="1:7">
@@ -13883,6 +13892,9 @@
       </c>
       <c r="E203" t="s">
         <v>500</v>
+      </c>
+      <c r="F203" t="s">
+        <v>1136</v>
       </c>
       <c r="G203"/>
     </row>

</xml_diff>

<commit_message>
updated rules spreadsheet for new rule added
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="1138">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5053,19 +5053,22 @@
     <t>testRule419ForAggravatedAssaultHomicideCircumstances</t>
   </si>
   <si>
-    <t>aae8824</t>
-  </si>
-  <si>
-    <t>b439de0</t>
-  </si>
-  <si>
-    <t>b1b8584</t>
-  </si>
-  <si>
-    <t>5bb1136</t>
-  </si>
-  <si>
-    <t>bdac265</t>
+    <t>factory test: 584fb9d</t>
+  </si>
+  <si>
+    <t>factory test: bdac265</t>
+  </si>
+  <si>
+    <t>factory test: 5bb1136</t>
+  </si>
+  <si>
+    <t>factory test:  b1b8584</t>
+  </si>
+  <si>
+    <t>factory test: b439de0</t>
+  </si>
+  <si>
+    <t>factory test:  aae8824</t>
   </si>
 </sst>
 </file>
@@ -9764,7 +9767,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="D203" sqref="D203"/>
+      <selection activeCell="F198" sqref="F198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13810,7 +13813,7 @@
         <v>500</v>
       </c>
       <c r="F199" t="s">
-        <v>1132</v>
+        <v>1137</v>
       </c>
       <c r="G199"/>
     </row>
@@ -13831,7 +13834,7 @@
         <v>500</v>
       </c>
       <c r="F200" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="G200"/>
     </row>
@@ -13852,7 +13855,7 @@
         <v>500</v>
       </c>
       <c r="F201" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="G201"/>
     </row>
@@ -13873,7 +13876,7 @@
         <v>500</v>
       </c>
       <c r="F202" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="G202"/>
     </row>
@@ -13894,7 +13897,7 @@
         <v>500</v>
       </c>
       <c r="F203" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="G203"/>
     </row>
@@ -13913,6 +13916,9 @@
       </c>
       <c r="E204" t="s">
         <v>500</v>
+      </c>
+      <c r="F204" t="s">
+        <v>1132</v>
       </c>
       <c r="G204"/>
     </row>

</xml_diff>

<commit_message>
updated spread sheet for new rule/test for sex of victim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2949" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2950" uniqueCount="1141">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5075,6 +5075,9 @@
   </si>
   <si>
     <t>rule and factory test:  204afc</t>
+  </si>
+  <si>
+    <t>rule and factory test: 9bee565</t>
   </si>
 </sst>
 </file>
@@ -9772,8 +9775,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="F206" sqref="C206:F206"/>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="F207" sqref="C207:F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13985,6 +13988,9 @@
       </c>
       <c r="E207" t="s">
         <v>500</v>
+      </c>
+      <c r="F207" t="s">
+        <v>1140</v>
       </c>
       <c r="G207"/>
     </row>

</xml_diff>

<commit_message>
updaed spreadsheet new rule: getRule455ForAdditionalJustifiableHomicideCircsumstances
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2950" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2952" uniqueCount="1143">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5078,6 +5078,12 @@
   </si>
   <si>
     <t>rule and factory test: 9bee565</t>
+  </si>
+  <si>
+    <t>rule and factory test:  4721da2</t>
+  </si>
+  <si>
+    <t>rule and factory test: 87381d6</t>
   </si>
 </sst>
 </file>
@@ -9776,7 +9782,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="F207" sqref="C207:F207"/>
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14010,6 +14016,9 @@
       <c r="E208" t="s">
         <v>500</v>
       </c>
+      <c r="F208" t="s">
+        <v>1141</v>
+      </c>
       <c r="G208"/>
     </row>
     <row r="209" spans="1:7" ht="42">
@@ -14027,6 +14036,9 @@
       </c>
       <c r="E209" t="s">
         <v>500</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1142</v>
       </c>
       <c r="G209"/>
     </row>

</xml_diff>

<commit_message>
updated rule spreadsheet for new rule: getRule457ForAdditionalJustifiableHomicideCircsumstances and factory test: testRule457ForAdditionalJustifiableHomicideCircsumstances
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2952" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="1144">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5084,6 +5084,9 @@
   </si>
   <si>
     <t>rule and factory test: 87381d6</t>
+  </si>
+  <si>
+    <t>rule and factory test: bbd9604</t>
   </si>
 </sst>
 </file>
@@ -9782,7 +9785,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="F210" sqref="F210"/>
+      <selection activeCell="F211" sqref="C211:F211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14075,6 +14078,9 @@
       </c>
       <c r="E211" t="s">
         <v>500</v>
+      </c>
+      <c r="F211" t="s">
+        <v>1143</v>
       </c>
       <c r="G211"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for new validation rule getRule458ForTypeOfInjury with its test
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1145">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5087,6 +5087,9 @@
   </si>
   <si>
     <t>rule and factory test: bbd9604</t>
+  </si>
+  <si>
+    <t>rule and factory test: 8e87630</t>
   </si>
 </sst>
 </file>
@@ -9784,8 +9787,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="F211" sqref="C211:F211"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="F212" sqref="C212:F212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14099,6 +14102,9 @@
       </c>
       <c r="E212" t="s">
         <v>500</v>
+      </c>
+      <c r="F212" t="s">
+        <v>1144</v>
       </c>
       <c r="G212"/>
     </row>

</xml_diff>

<commit_message>
updated nibrs validation spreadsheet for new test: testRule458ForEthnicityOfVictim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="1146">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5090,6 +5090,9 @@
   </si>
   <si>
     <t>rule and factory test: 8e87630</t>
+  </si>
+  <si>
+    <t>rule and factory test: 5142917</t>
   </si>
 </sst>
 </file>
@@ -9787,8 +9790,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="F212" sqref="C212:F212"/>
+    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F214" sqref="F214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14123,6 +14126,9 @@
       </c>
       <c r="E213" t="s">
         <v>500</v>
+      </c>
+      <c r="F213" t="s">
+        <v>1145</v>
       </c>
       <c r="G213"/>
     </row>

</xml_diff>

<commit_message>
updated spreadseet for validation test: testRule458ForResidentStatusOfVictim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="1147">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5093,6 +5093,9 @@
   </si>
   <si>
     <t>rule and factory test: 5142917</t>
+  </si>
+  <si>
+    <t>rule update and factory tes: 68b5a58</t>
   </si>
 </sst>
 </file>
@@ -9791,7 +9794,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F214" sqref="F214"/>
+      <selection activeCell="C214" sqref="C214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14147,6 +14150,9 @@
       </c>
       <c r="E214" t="s">
         <v>500</v>
+      </c>
+      <c r="F214" t="s">
+        <v>1146</v>
       </c>
       <c r="G214"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for validation rule test of: testRule458ForOffenderNumberToBeRelated
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="1148">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5095,7 +5095,10 @@
     <t>rule and factory test: 5142917</t>
   </si>
   <si>
-    <t>rule update and factory tes: 68b5a58</t>
+    <t>rule update and factory test: 68b5a58</t>
+  </si>
+  <si>
+    <t>rule update and factory test: 3da18d1</t>
   </si>
 </sst>
 </file>
@@ -9794,7 +9797,7 @@
   <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C214" sqref="C214"/>
+      <selection activeCell="F215" sqref="F215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14171,6 +14174,9 @@
       </c>
       <c r="E215" t="s">
         <v>500</v>
+      </c>
+      <c r="F215" t="s">
+        <v>1147</v>
       </c>
       <c r="G215"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with test: testRule458ForSexOfVictim and rule: getRule458ForSexOfVictim
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="1148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="1149">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5099,6 +5099,9 @@
   </si>
   <si>
     <t>rule update and factory test: 3da18d1</t>
+  </si>
+  <si>
+    <t>rule update and factory test: 811d6cb</t>
   </si>
 </sst>
 </file>
@@ -9796,8 +9799,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F215" sqref="F215"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F217" sqref="F217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14195,6 +14198,9 @@
       </c>
       <c r="E216" t="s">
         <v>500</v>
+      </c>
+      <c r="F216" t="s">
+        <v>1148</v>
       </c>
       <c r="G216"/>
     </row>

</xml_diff>

<commit_message>
Updated tracking spreadsheet with offender segment updates
</commit_message>
<xml_diff>
--- a/docs/NIBRSEditRules.xlsx
+++ b/docs/NIBRSEditRules.xlsx
@@ -15,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ElementEdits!$A$1:$G$345</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Rules!$A$1:$E$251</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1181">
   <si>
     <t>RuleNumber</t>
   </si>
@@ -5162,6 +5162,42 @@
   </si>
   <si>
     <t>8ce0016</t>
+  </si>
+  <si>
+    <t>89bebb1</t>
+  </si>
+  <si>
+    <t>2400e66</t>
+  </si>
+  <si>
+    <t>N/A - handled in importer creation of NIBRSAge</t>
+  </si>
+  <si>
+    <t>c540d1b</t>
+  </si>
+  <si>
+    <t>14710ee</t>
+  </si>
+  <si>
+    <t>779b725</t>
+  </si>
+  <si>
+    <t>666195a</t>
+  </si>
+  <si>
+    <t>Note - this rule is being removed by FBI</t>
+  </si>
+  <si>
+    <t>5f85223</t>
+  </si>
+  <si>
+    <t>67546bd</t>
+  </si>
+  <si>
+    <t>1cd6048</t>
+  </si>
+  <si>
+    <t>0d2cd2e</t>
   </si>
 </sst>
 </file>
@@ -9859,8 +9895,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F188" sqref="F188"/>
+    <sheetView tabSelected="1" topLeftCell="A255" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F346" sqref="F346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13223,7 +13259,7 @@
       </c>
       <c r="G166"/>
     </row>
-    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>496</v>
       </c>
@@ -13244,7 +13280,7 @@
       </c>
       <c r="G167"/>
     </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>501</v>
       </c>
@@ -13265,7 +13301,7 @@
       </c>
       <c r="G168"/>
     </row>
-    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>656</v>
       </c>
@@ -13286,7 +13322,7 @@
       </c>
       <c r="G169"/>
     </row>
-    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>758</v>
       </c>
@@ -13307,7 +13343,7 @@
       </c>
       <c r="G170"/>
     </row>
-    <row r="171" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>794</v>
       </c>
@@ -13328,7 +13364,7 @@
       </c>
       <c r="G171"/>
     </row>
-    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>508</v>
       </c>
@@ -13349,7 +13385,7 @@
       </c>
       <c r="G172"/>
     </row>
-    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>528</v>
       </c>
@@ -13370,7 +13406,7 @@
       </c>
       <c r="G173"/>
     </row>
-    <row r="174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>532</v>
       </c>
@@ -13391,7 +13427,7 @@
       </c>
       <c r="G174"/>
     </row>
-    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>536</v>
       </c>
@@ -13412,7 +13448,7 @@
       </c>
       <c r="G175"/>
     </row>
-    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>550</v>
       </c>
@@ -13433,7 +13469,7 @@
       </c>
       <c r="G176"/>
     </row>
-    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>656</v>
       </c>
@@ -13454,7 +13490,7 @@
       </c>
       <c r="G177"/>
     </row>
-    <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>807</v>
       </c>
@@ -13475,7 +13511,7 @@
       </c>
       <c r="G178"/>
     </row>
-    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>813</v>
       </c>
@@ -13496,7 +13532,7 @@
       </c>
       <c r="G179"/>
     </row>
-    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>818</v>
       </c>
@@ -13517,7 +13553,7 @@
       </c>
       <c r="G180"/>
     </row>
-    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>823</v>
       </c>
@@ -13538,7 +13574,7 @@
       </c>
       <c r="G181"/>
     </row>
-    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>831</v>
       </c>
@@ -13559,7 +13595,7 @@
       </c>
       <c r="G182"/>
     </row>
-    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>860</v>
       </c>
@@ -13580,7 +13616,7 @@
       </c>
       <c r="G183"/>
     </row>
-    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>867</v>
       </c>
@@ -13601,7 +13637,7 @@
       </c>
       <c r="G184"/>
     </row>
-    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>877</v>
       </c>
@@ -13622,7 +13658,7 @@
       </c>
       <c r="G185"/>
     </row>
-    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>501</v>
       </c>
@@ -13643,7 +13679,7 @@
       </c>
       <c r="G186"/>
     </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>536</v>
       </c>
@@ -13664,7 +13700,7 @@
       </c>
       <c r="G187"/>
     </row>
-    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>550</v>
       </c>
@@ -13685,7 +13721,7 @@
       </c>
       <c r="G188"/>
     </row>
-    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>867</v>
       </c>
@@ -13706,7 +13742,7 @@
       </c>
       <c r="G189"/>
     </row>
-    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>867</v>
       </c>
@@ -13727,7 +13763,7 @@
       </c>
       <c r="G190"/>
     </row>
-    <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>508</v>
       </c>
@@ -13748,7 +13784,7 @@
       </c>
       <c r="G191"/>
     </row>
-    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>508</v>
       </c>
@@ -13769,7 +13805,7 @@
       </c>
       <c r="G192"/>
     </row>
-    <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>508</v>
       </c>
@@ -13790,7 +13826,7 @@
       </c>
       <c r="G193"/>
     </row>
-    <row r="194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>758</v>
       </c>
@@ -13811,7 +13847,7 @@
       </c>
       <c r="G194"/>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>758</v>
       </c>
@@ -13832,7 +13868,7 @@
       </c>
       <c r="G195"/>
     </row>
-    <row r="196" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>758</v>
       </c>
@@ -13853,7 +13889,7 @@
       </c>
       <c r="G196"/>
     </row>
-    <row r="197" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>536</v>
       </c>
@@ -13874,7 +13910,7 @@
       </c>
       <c r="G197"/>
     </row>
-    <row r="198" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>867</v>
       </c>
@@ -13892,7 +13928,7 @@
       </c>
       <c r="G198"/>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>508</v>
       </c>
@@ -13913,7 +13949,7 @@
       </c>
       <c r="G199"/>
     </row>
-    <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>508</v>
       </c>
@@ -13934,7 +13970,7 @@
       </c>
       <c r="G200"/>
     </row>
-    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>508</v>
       </c>
@@ -13955,7 +13991,7 @@
       </c>
       <c r="G201"/>
     </row>
-    <row r="202" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>823</v>
       </c>
@@ -13976,7 +14012,7 @@
       </c>
       <c r="G202"/>
     </row>
-    <row r="203" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>831</v>
       </c>
@@ -13997,7 +14033,7 @@
       </c>
       <c r="G203"/>
     </row>
-    <row r="204" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>508</v>
       </c>
@@ -14018,7 +14054,7 @@
       </c>
       <c r="G204"/>
     </row>
-    <row r="205" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>807</v>
       </c>
@@ -14039,7 +14075,7 @@
       </c>
       <c r="G205"/>
     </row>
-    <row r="206" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>813</v>
       </c>
@@ -14060,7 +14096,7 @@
       </c>
       <c r="G206"/>
     </row>
-    <row r="207" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>823</v>
       </c>
@@ -14081,7 +14117,7 @@
       </c>
       <c r="G207"/>
     </row>
-    <row r="208" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>831</v>
       </c>
@@ -14102,7 +14138,7 @@
       </c>
       <c r="G208"/>
     </row>
-    <row r="209" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>860</v>
       </c>
@@ -14123,7 +14159,7 @@
       </c>
       <c r="G209"/>
     </row>
-    <row r="210" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>536</v>
       </c>
@@ -14144,7 +14180,7 @@
       </c>
       <c r="G210"/>
     </row>
-    <row r="211" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>860</v>
       </c>
@@ -14165,7 +14201,7 @@
       </c>
       <c r="G211"/>
     </row>
-    <row r="212" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>508</v>
       </c>
@@ -14186,7 +14222,7 @@
       </c>
       <c r="G212"/>
     </row>
-    <row r="213" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>528</v>
       </c>
@@ -14207,7 +14243,7 @@
       </c>
       <c r="G213"/>
     </row>
-    <row r="214" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>532</v>
       </c>
@@ -14228,7 +14264,7 @@
       </c>
       <c r="G214"/>
     </row>
-    <row r="215" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>550</v>
       </c>
@@ -14249,7 +14285,7 @@
       </c>
       <c r="G215"/>
     </row>
-    <row r="216" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>823</v>
       </c>
@@ -14270,7 +14306,7 @@
       </c>
       <c r="G216"/>
     </row>
-    <row r="217" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>831</v>
       </c>
@@ -14291,7 +14327,7 @@
       </c>
       <c r="G217"/>
     </row>
-    <row r="218" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>867</v>
       </c>
@@ -14312,7 +14348,7 @@
       </c>
       <c r="G218"/>
     </row>
-    <row r="219" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>550</v>
       </c>
@@ -14333,7 +14369,7 @@
       </c>
       <c r="G219"/>
     </row>
-    <row r="220" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>877</v>
       </c>
@@ -14354,7 +14390,7 @@
       </c>
       <c r="G220"/>
     </row>
-    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>794</v>
       </c>
@@ -14375,7 +14411,7 @@
       </c>
       <c r="G221"/>
     </row>
-    <row r="222" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>536</v>
       </c>
@@ -14396,7 +14432,7 @@
       </c>
       <c r="G222"/>
     </row>
-    <row r="223" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>536</v>
       </c>
@@ -14417,7 +14453,7 @@
       </c>
       <c r="G223"/>
     </row>
-    <row r="224" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>794</v>
       </c>
@@ -14438,7 +14474,7 @@
       </c>
       <c r="G224"/>
     </row>
-    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>794</v>
       </c>
@@ -14459,7 +14495,7 @@
       </c>
       <c r="G225"/>
     </row>
-    <row r="226" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>794</v>
       </c>
@@ -14480,7 +14516,7 @@
       </c>
       <c r="G226"/>
     </row>
-    <row r="227" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>877</v>
       </c>
@@ -14501,7 +14537,7 @@
       </c>
       <c r="G227"/>
     </row>
-    <row r="228" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>823</v>
       </c>
@@ -14522,7 +14558,7 @@
       </c>
       <c r="G228"/>
     </row>
-    <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>550</v>
       </c>
@@ -14543,7 +14579,7 @@
       </c>
       <c r="G229"/>
     </row>
-    <row r="230" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>877</v>
       </c>
@@ -14564,7 +14600,7 @@
       </c>
       <c r="G230"/>
     </row>
-    <row r="231" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>550</v>
       </c>
@@ -14585,7 +14621,7 @@
       </c>
       <c r="G231"/>
     </row>
-    <row r="232" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>536</v>
       </c>
@@ -14606,7 +14642,7 @@
       </c>
       <c r="G232"/>
     </row>
-    <row r="233" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>501</v>
       </c>
@@ -14627,7 +14663,7 @@
       </c>
       <c r="G233"/>
     </row>
-    <row r="234" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>867</v>
       </c>
@@ -14648,7 +14684,7 @@
       </c>
       <c r="G234"/>
     </row>
-    <row r="235" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>508</v>
       </c>
@@ -14669,7 +14705,7 @@
       </c>
       <c r="G235"/>
     </row>
-    <row r="236" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>794</v>
       </c>
@@ -14690,7 +14726,7 @@
       </c>
       <c r="G236"/>
     </row>
-    <row r="237" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>807</v>
       </c>
@@ -14711,7 +14747,7 @@
       </c>
       <c r="G237"/>
     </row>
-    <row r="238" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>813</v>
       </c>
@@ -14732,7 +14768,7 @@
       </c>
       <c r="G238"/>
     </row>
-    <row r="239" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>818</v>
       </c>
@@ -14753,7 +14789,7 @@
       </c>
       <c r="G239"/>
     </row>
-    <row r="240" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>656</v>
       </c>
@@ -14769,9 +14805,12 @@
       <c r="E240" t="s">
         <v>565</v>
       </c>
+      <c r="F240" t="s">
+        <v>984</v>
+      </c>
       <c r="G240"/>
     </row>
-    <row r="241" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>758</v>
       </c>
@@ -14787,9 +14826,12 @@
       <c r="E241" t="s">
         <v>565</v>
       </c>
+      <c r="F241" t="s">
+        <v>984</v>
+      </c>
       <c r="G241"/>
     </row>
-    <row r="242" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>886</v>
       </c>
@@ -14805,9 +14847,12 @@
       <c r="E242" t="s">
         <v>565</v>
       </c>
+      <c r="F242" t="s">
+        <v>1169</v>
+      </c>
       <c r="G242"/>
     </row>
-    <row r="243" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>561</v>
       </c>
@@ -14823,9 +14868,12 @@
       <c r="E243" t="s">
         <v>565</v>
       </c>
+      <c r="F243" t="s">
+        <v>1169</v>
+      </c>
       <c r="G243"/>
     </row>
-    <row r="244" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>656</v>
       </c>
@@ -14841,9 +14889,12 @@
       <c r="E244" t="s">
         <v>565</v>
       </c>
+      <c r="F244" t="s">
+        <v>984</v>
+      </c>
       <c r="G244"/>
     </row>
-    <row r="245" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>891</v>
       </c>
@@ -14859,9 +14910,12 @@
       <c r="E245" t="s">
         <v>565</v>
       </c>
+      <c r="F245" s="9" t="s">
+        <v>1170</v>
+      </c>
       <c r="G245"/>
     </row>
-    <row r="246" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>897</v>
       </c>
@@ -14877,9 +14931,12 @@
       <c r="E246" t="s">
         <v>565</v>
       </c>
+      <c r="F246" s="9" t="s">
+        <v>1170</v>
+      </c>
       <c r="G246"/>
     </row>
-    <row r="247" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>903</v>
       </c>
@@ -14895,9 +14952,12 @@
       <c r="E247" t="s">
         <v>565</v>
       </c>
+      <c r="F247" s="9" t="s">
+        <v>1170</v>
+      </c>
       <c r="G247"/>
     </row>
-    <row r="248" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>561</v>
       </c>
@@ -14913,9 +14973,12 @@
       <c r="E248" t="s">
         <v>565</v>
       </c>
+      <c r="F248" s="8" t="s">
+        <v>1171</v>
+      </c>
       <c r="G248"/>
     </row>
-    <row r="249" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>561</v>
       </c>
@@ -14931,9 +14994,12 @@
       <c r="E249" t="s">
         <v>565</v>
       </c>
+      <c r="F249" s="8" t="s">
+        <v>1171</v>
+      </c>
       <c r="G249"/>
     </row>
-    <row r="250" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>561</v>
       </c>
@@ -14949,9 +15015,12 @@
       <c r="E250" t="s">
         <v>565</v>
       </c>
+      <c r="F250" s="8" t="s">
+        <v>1172</v>
+      </c>
       <c r="G250"/>
     </row>
-    <row r="251" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>758</v>
       </c>
@@ -14967,9 +15036,12 @@
       <c r="E251" t="s">
         <v>565</v>
       </c>
+      <c r="F251" s="8" t="s">
+        <v>984</v>
+      </c>
       <c r="G251"/>
     </row>
-    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>758</v>
       </c>
@@ -14985,9 +15057,12 @@
       <c r="E252" t="s">
         <v>565</v>
       </c>
+      <c r="F252" s="8" t="s">
+        <v>984</v>
+      </c>
       <c r="G252"/>
     </row>
-    <row r="253" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>758</v>
       </c>
@@ -15003,9 +15078,12 @@
       <c r="E253" t="s">
         <v>565</v>
       </c>
+      <c r="F253" s="8" t="s">
+        <v>984</v>
+      </c>
       <c r="G253"/>
     </row>
-    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>561</v>
       </c>
@@ -15021,9 +15099,12 @@
       <c r="E254" t="s">
         <v>565</v>
       </c>
+      <c r="F254" s="8" t="s">
+        <v>1173</v>
+      </c>
       <c r="G254"/>
     </row>
-    <row r="255" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>561</v>
       </c>
@@ -15039,9 +15120,12 @@
       <c r="E255" t="s">
         <v>565</v>
       </c>
+      <c r="F255" s="8" t="s">
+        <v>1174</v>
+      </c>
       <c r="G255"/>
     </row>
-    <row r="256" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>561</v>
       </c>
@@ -15057,9 +15141,12 @@
       <c r="E256" t="s">
         <v>565</v>
       </c>
+      <c r="F256" s="8" t="s">
+        <v>1175</v>
+      </c>
       <c r="G256"/>
     </row>
-    <row r="257" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>891</v>
       </c>
@@ -15075,9 +15162,12 @@
       <c r="E257" t="s">
         <v>565</v>
       </c>
+      <c r="F257" s="8" t="s">
+        <v>1175</v>
+      </c>
       <c r="G257"/>
     </row>
-    <row r="258" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>897</v>
       </c>
@@ -15093,9 +15183,12 @@
       <c r="E258" t="s">
         <v>565</v>
       </c>
+      <c r="F258" s="8" t="s">
+        <v>1175</v>
+      </c>
       <c r="G258"/>
     </row>
-    <row r="259" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>903</v>
       </c>
@@ -15111,9 +15204,12 @@
       <c r="E259" t="s">
         <v>565</v>
       </c>
+      <c r="F259" s="8" t="s">
+        <v>1175</v>
+      </c>
       <c r="G259"/>
     </row>
-    <row r="260" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>891</v>
       </c>
@@ -15129,9 +15225,14 @@
       <c r="E260" t="s">
         <v>565</v>
       </c>
-      <c r="G260"/>
-    </row>
-    <row r="261" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F260" s="8" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G260" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>561</v>
       </c>
@@ -15147,9 +15248,12 @@
       <c r="E261" t="s">
         <v>565</v>
       </c>
+      <c r="F261" s="8" t="s">
+        <v>1178</v>
+      </c>
       <c r="G261"/>
     </row>
-    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>561</v>
       </c>
@@ -15165,9 +15269,12 @@
       <c r="E262" t="s">
         <v>565</v>
       </c>
+      <c r="F262" s="8" t="s">
+        <v>1179</v>
+      </c>
       <c r="G262"/>
     </row>
-    <row r="263" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>886</v>
       </c>
@@ -15183,9 +15290,12 @@
       <c r="E263" t="s">
         <v>565</v>
       </c>
+      <c r="F263" t="s">
+        <v>1169</v>
+      </c>
       <c r="G263"/>
     </row>
-    <row r="264" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>897</v>
       </c>
@@ -15200,6 +15310,9 @@
       </c>
       <c r="E264" t="s">
         <v>565</v>
+      </c>
+      <c r="F264" s="8" t="s">
+        <v>1180</v>
       </c>
       <c r="G264"/>
     </row>
@@ -16665,7 +16778,7 @@
   <autoFilter ref="A1:G345">
     <filterColumn colId="4">
       <filters>
-        <filter val="4"/>
+        <filter val="5"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:G345">

</xml_diff>